<commit_message>
Update default place create forms after merge
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
   <si>
     <t>type</t>
   </si>
@@ -209,7 +209,7 @@
     <t>custom_place_name_label_translator</t>
   </si>
   <si>
-    <t>selected(${create_new_person},'none')</t>
+    <t xml:space="preserve">selected(${create_new_person},'none') or selected(${is_name_generated}, 'false')</t>
   </si>
   <si>
     <t>"name"</t>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>${custom_place_name_label}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(${create_new_person},'none') or selected(${is_name_generated}, 'false')  or selected(${is_name_generated}, 'no')</t>
   </si>
   <si>
     <t xml:space="preserve">Standalone question only if no contact is selected, so show label accordingly</t>
@@ -1158,7 +1155,7 @@
   <fonts count="5">
     <font>
       <name val="Calibri"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <sz val="11.000000"/>
     </font>
     <font>
@@ -1168,7 +1165,6 @@
     <font>
       <name val="Calibri"/>
       <b/>
-      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
     <font>
@@ -1177,7 +1173,6 @@
     </font>
     <font>
       <name val="Arial"/>
-      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
   </fonts>
@@ -1292,9 +1287,9 @@
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2687,7 +2682,7 @@
         <v>28</v>
       </c>
       <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="19" t="s">
         <v>64</v>
       </c>
       <c r="L15" s="16" t="s">
@@ -2809,8 +2804,8 @@
       <c r="J17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>70</v>
+      <c r="K17" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="L17" s="16"/>
       <c r="M17" s="16"/>
@@ -2827,7 +2822,7 @@
       <c r="X17" s="16"/>
       <c r="Y17" s="16"/>
       <c r="Z17" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA17" s="16"/>
       <c r="AB17" s="16"/>
@@ -2850,29 +2845,29 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>78</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
@@ -2892,7 +2887,7 @@
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
       <c r="Y18" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z18" s="16"/>
       <c r="AA18" s="16"/>
@@ -2919,7 +2914,7 @@
         <v>59</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -2935,7 +2930,7 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
       <c r="P19" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
@@ -2968,10 +2963,10 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>84</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>28</v>
@@ -3010,7 +3005,7 @@
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
       <c r="Y20" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z20" s="16"/>
       <c r="AA20" s="16"/>
@@ -3037,7 +3032,7 @@
         <v>59</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -3053,7 +3048,7 @@
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
       <c r="P21" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
@@ -3177,30 +3172,30 @@
         <v>26</v>
       </c>
       <c r="B24" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="D24" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="E24" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="F24" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>91</v>
-      </c>
       <c r="G24" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>38</v>
@@ -3243,7 +3238,7 @@
         <v>58</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>28</v>
@@ -3260,7 +3255,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3280,7 +3275,7 @@
       <c r="W25" s="16"/>
       <c r="X25" s="16"/>
       <c r="Y25" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z25" s="16"/>
       <c r="AA25" s="16"/>
@@ -3324,7 +3319,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="19"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3344,7 +3339,7 @@
       <c r="W26" s="16"/>
       <c r="X26" s="16"/>
       <c r="Y26" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Z26" s="16"/>
       <c r="AA26" s="16"/>
@@ -3374,23 +3369,23 @@
         <v>1</v>
       </c>
       <c r="C27" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="E27" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="F27" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="G27" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J27" s="16" t="s">
         <v>47</v>
@@ -3399,7 +3394,7 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
@@ -3437,10 +3432,10 @@
         <v>30</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>103</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>104</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -3449,21 +3444,21 @@
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
       <c r="J28" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
       <c r="N28" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="O28" s="16" t="s">
         <v>106</v>
-      </c>
-      <c r="O28" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="20" t="s">
-        <v>108</v>
+      <c r="R28" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="S28" s="16"/>
       <c r="T28" s="16"/>
@@ -3497,9 +3492,9 @@
         <v>59</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="19"/>
+        <v>108</v>
+      </c>
+      <c r="C29" s="20"/>
       <c r="D29" s="18"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -3515,7 +3510,7 @@
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
       <c r="P29" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
@@ -3551,9 +3546,9 @@
         <v>59</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="19"/>
+        <v>110</v>
+      </c>
+      <c r="C30" s="20"/>
       <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -3567,7 +3562,7 @@
       <c r="N30" s="16"/>
       <c r="O30" s="16"/>
       <c r="P30" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
@@ -3603,25 +3598,25 @@
         <v>26</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19" t="s">
+      <c r="H31" s="20"/>
+      <c r="I31" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J31" s="16"/>
@@ -3662,13 +3657,13 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="16"/>
@@ -3680,20 +3675,20 @@
         <v>47</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="O32" s="16" t="s">
         <v>118</v>
-      </c>
-      <c r="O32" s="16" t="s">
-        <v>119</v>
       </c>
       <c r="P32" s="16"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S32" s="16"/>
       <c r="T32" s="16"/>
@@ -3724,13 +3719,13 @@
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -3740,7 +3735,7 @@
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
       <c r="K33" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
@@ -3778,13 +3773,13 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="16"/>
@@ -3796,15 +3791,15 @@
         <v>47</v>
       </c>
       <c r="K34" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="O34" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="O34" s="16" t="s">
-        <v>129</v>
       </c>
       <c r="P34" s="16"/>
       <c r="Q34" s="16"/>
@@ -3838,13 +3833,13 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>130</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="16"/>
@@ -3854,15 +3849,15 @@
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
       <c r="K35" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="O35" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="O35" s="16" t="s">
-        <v>133</v>
       </c>
       <c r="P35" s="16"/>
       <c r="Q35" s="16"/>
@@ -3896,13 +3891,13 @@
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="C36" s="16" t="s">
         <v>135</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>136</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="16"/>
@@ -3913,7 +3908,7 @@
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
       <c r="L36" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
@@ -3953,7 +3948,7 @@
         <v>59</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" s="16"/>
       <c r="D37" s="18"/>
@@ -3968,8 +3963,8 @@
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="21" t="s">
-        <v>139</v>
+      <c r="P37" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -4005,7 +4000,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="18"/>
@@ -4020,8 +4015,8 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="21" t="s">
-        <v>141</v>
+      <c r="P38" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
@@ -4057,10 +4052,10 @@
         <v>59</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>142</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>143</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="16"/>
@@ -4075,7 +4070,7 @@
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
       <c r="P39" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
@@ -4111,7 +4106,7 @@
         <v>59</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="18"/>
@@ -4127,7 +4122,7 @@
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
       <c r="P40" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
@@ -4163,10 +4158,10 @@
         <v>59</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="16"/>
@@ -4181,7 +4176,7 @@
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
       <c r="P41" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
@@ -4214,13 +4209,13 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>149</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>150</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="16"/>
@@ -4317,33 +4312,33 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="D44" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="E44" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="F44" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="G44" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="G44" s="16" t="s">
-        <v>157</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J44" s="16"/>
       <c r="K44" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L44" s="16"/>
       <c r="M44" s="16"/>
@@ -4352,7 +4347,7 @@
         <v>1</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
@@ -4386,33 +4381,33 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B45" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="D45" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="E45" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="F45" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="G45" s="16" t="s">
         <v>164</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>165</v>
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J45" s="16"/>
       <c r="K45" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
@@ -4421,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
@@ -4455,38 +4450,38 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="D46" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="E46" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="F46" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="F46" s="16" t="s">
-        <v>172</v>
-      </c>
       <c r="G46" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
@@ -4523,33 +4518,33 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="C47" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="D47" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="E47" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="F47" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="G47" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>180</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
@@ -4590,32 +4585,32 @@
         <v>30</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="D48" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="E48" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="F48" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="G48" s="16" t="s">
         <v>186</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>187</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L48" s="16"/>
       <c r="M48" s="16"/>
@@ -4656,30 +4651,30 @@
         <v>30</v>
       </c>
       <c r="B49" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="E49" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="F49" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="G49" s="16" t="s">
         <v>194</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>195</v>
       </c>
       <c r="H49" s="16"/>
       <c r="I49" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J49" s="16"/>
       <c r="K49" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
@@ -4723,30 +4718,30 @@
         <v>25</v>
       </c>
       <c r="C50" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="E50" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="F50" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F50" s="16" t="s">
+      <c r="G50" s="16" t="s">
         <v>200</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>201</v>
       </c>
       <c r="H50" s="16"/>
       <c r="I50" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J50" s="16"/>
       <c r="K50" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L50" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
@@ -4786,7 +4781,7 @@
         <v>26</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>28</v>
@@ -4840,7 +4835,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -4856,7 +4851,7 @@
       <c r="N52" s="16"/>
       <c r="O52" s="16"/>
       <c r="P52" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
@@ -4892,7 +4887,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
@@ -4908,7 +4903,7 @@
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
       <c r="P53" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
@@ -4944,7 +4939,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
@@ -4960,7 +4955,7 @@
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
       <c r="P54" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
@@ -5132,7 +5127,7 @@
         <v>26</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>28</v>
@@ -5196,7 +5191,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C59" s="16" t="s">
         <v>28</v>
@@ -5233,7 +5228,7 @@
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
       <c r="Y59" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z59" s="16"/>
       <c r="AA59" s="16"/>
@@ -5319,35 +5314,35 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B61" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="C61" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="D61" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="E61" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="F61" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="F61" s="16" t="s">
+      <c r="G61" s="16" t="s">
         <v>215</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>216</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J61" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K61" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L61" s="16" t="s">
         <v>48</v>
@@ -5365,7 +5360,7 @@
       <c r="W61" s="16"/>
       <c r="X61" s="16"/>
       <c r="Y61" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Z61" s="16"/>
       <c r="AA61" s="16"/>
@@ -5395,23 +5390,23 @@
         <v>1</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D62" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="F62" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F62" s="16" t="s">
-        <v>100</v>
-      </c>
       <c r="G62" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J62" s="16" t="s">
         <v>47</v>
@@ -5422,7 +5417,7 @@
       <c r="N62" s="16"/>
       <c r="O62" s="22"/>
       <c r="P62" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q62" s="16"/>
       <c r="R62" s="16"/>
@@ -5458,26 +5453,26 @@
         <v>30</v>
       </c>
       <c r="B63" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C63" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="D63" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="E63" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="E63" s="16" t="s">
-        <v>193</v>
-      </c>
       <c r="F63" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H63" s="16"/>
       <c r="I63" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
@@ -5523,28 +5518,28 @@
         <v>25</v>
       </c>
       <c r="C64" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="E64" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="F64" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F64" s="16" t="s">
+      <c r="G64" s="18" t="s">
         <v>200</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>201</v>
       </c>
       <c r="H64" s="16"/>
       <c r="I64" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
       <c r="L64" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
@@ -5584,7 +5579,7 @@
         <v>59</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="16"/>
       <c r="D65" s="16"/>
@@ -5600,7 +5595,7 @@
       <c r="N65" s="16"/>
       <c r="O65" s="16"/>
       <c r="P65" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q65" s="16"/>
       <c r="R65" s="16"/>
@@ -5636,7 +5631,7 @@
         <v>59</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
@@ -5652,7 +5647,7 @@
       <c r="N66" s="16"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
@@ -5688,7 +5683,7 @@
         <v>26</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C67" s="16" t="s">
         <v>28</v>
@@ -5752,7 +5747,7 @@
         <v>59</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C68" s="16"/>
       <c r="D68" s="16"/>
@@ -5768,7 +5763,7 @@
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
       <c r="P68" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q68" s="16"/>
       <c r="R68" s="16"/>
@@ -5804,7 +5799,7 @@
         <v>59</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
@@ -5820,7 +5815,7 @@
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
       <c r="P69" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
@@ -5856,7 +5851,7 @@
         <v>59</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
@@ -5872,7 +5867,7 @@
       <c r="N70" s="16"/>
       <c r="O70" s="16"/>
       <c r="P70" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q70" s="16"/>
       <c r="R70" s="16"/>
@@ -6033,7 +6028,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6079,29 +6074,29 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="G2" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="20" t="s">
         <v>232</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="19" t="s">
-        <v>233</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -6123,29 +6118,29 @@
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="G3" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="19" t="s">
-        <v>240</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6167,29 +6162,29 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="D4" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="E4" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="F4" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="G4" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="20" t="s">
         <v>247</v>
-      </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="19" t="s">
-        <v>248</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -6211,29 +6206,29 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B5" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="D5" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="F5" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="G5" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="20" t="s">
         <v>254</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="19" t="s">
-        <v>255</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -6255,29 +6250,29 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="D6" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="E6" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="F6" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="G6" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="20" t="s">
         <v>261</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -6299,29 +6294,29 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="D7" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="F7" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="G7" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="20" t="s">
         <v>268</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="19" t="s">
-        <v>269</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -6343,29 +6338,29 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>270</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="D8" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="E8" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="F8" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="G8" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="H8" s="30"/>
+      <c r="I8" s="20" t="s">
         <v>275</v>
-      </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="19" t="s">
-        <v>276</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -6387,20 +6382,20 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="33" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="C9" s="34" t="s">
         <v>278</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>279</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="32"/>
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -6421,29 +6416,29 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" s="33" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="C10" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="D10" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="E10" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="F10" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="G10" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="H10" s="30"/>
+      <c r="I10" s="20" t="s">
         <v>286</v>
-      </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="19" t="s">
-        <v>287</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -6465,29 +6460,29 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B11" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="D11" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="F11" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="G11" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="H11" s="30"/>
+      <c r="I11" s="20" t="s">
         <v>293</v>
-      </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="19" t="s">
-        <v>294</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -6509,29 +6504,29 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="D12" s="27" t="s">
         <v>296</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="F12" s="28" t="s">
         <v>298</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="G12" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="20" t="s">
         <v>299</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>297</v>
-      </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="19" t="s">
-        <v>300</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6553,29 +6548,29 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B13" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="D13" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="E13" s="32" t="s">
         <v>303</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="F13" s="28" t="s">
         <v>304</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="G13" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="20" t="s">
         <v>306</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="19" t="s">
-        <v>307</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -6597,29 +6592,29 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="27" t="s">
         <v>309</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="E14" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="F14" s="28" t="s">
         <v>311</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="G14" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="G14" s="29" t="s">
-        <v>313</v>
-      </c>
       <c r="H14" s="30"/>
-      <c r="I14" s="19" t="s">
-        <v>309</v>
+      <c r="I14" s="20" t="s">
+        <v>308</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -6641,29 +6636,29 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B15" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="D15" s="27" t="s">
         <v>315</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="E15" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="F15" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="G15" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="20" t="s">
         <v>318</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="19" t="s">
-        <v>319</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -6685,29 +6680,29 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>320</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>321</v>
-      </c>
       <c r="H16" s="30"/>
-      <c r="I16" s="19" t="s">
-        <v>233</v>
+      <c r="I16" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -6729,29 +6724,29 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="E17" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="F17" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="G17" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="H17" s="30"/>
+      <c r="I17" s="20" t="s">
         <v>326</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="19" t="s">
-        <v>327</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -6773,29 +6768,29 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="D18" s="27" t="s">
         <v>329</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="E18" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="F18" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="G18" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="20" t="s">
         <v>333</v>
-      </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="19" t="s">
-        <v>334</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6817,29 +6812,29 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="D19" s="27" t="s">
         <v>336</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="E19" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="F19" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="G19" s="29" t="s">
         <v>339</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="20" t="s">
         <v>340</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="19" t="s">
-        <v>341</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6861,29 +6856,29 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="27" t="s">
         <v>343</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="E20" s="32" t="s">
         <v>344</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="F20" s="28" t="s">
         <v>345</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="G20" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="20" t="s">
         <v>346</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>344</v>
-      </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="19" t="s">
-        <v>347</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6905,29 +6900,29 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C21" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>348</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="E21" s="32" t="s">
         <v>349</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="F21" s="28" t="s">
         <v>350</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="G21" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="H21" s="30"/>
+      <c r="I21" s="20" t="s">
         <v>352</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="19" t="s">
-        <v>353</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6949,29 +6944,29 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C22" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>354</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="E22" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="F22" s="28" t="s">
         <v>356</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="G22" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="H22" s="30"/>
+      <c r="I22" s="20" t="s">
         <v>358</v>
-      </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="19" t="s">
-        <v>359</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -6993,29 +6988,29 @@
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C23" s="34" t="s">
+        <v>359</v>
+      </c>
+      <c r="D23" s="27" t="s">
         <v>360</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="E23" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="F23" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="G23" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="H23" s="30"/>
+      <c r="I23" s="20" t="s">
         <v>364</v>
-      </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="19" t="s">
-        <v>365</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -7037,29 +7032,29 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="36" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B24" s="33" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D24" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="F24" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="G24" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="30"/>
+      <c r="I24" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="30"/>
-      <c r="I24" s="19" t="s">
-        <v>101</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -7113,19 +7108,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7150,20 +7145,20 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>373</v>
       </c>
       <c r="C2" s="37" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-02-24 13-11</v>
+        <v xml:space="preserve">2022-03-11 17-37</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>374</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>375</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>

</xml_diff>

<commit_message>
Fix dob_approx calculations in default forms
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -446,7 +446,7 @@
     <t>DOB</t>
   </si>
   <si>
-    <t xml:space="preserve">concat(string(${ephemeral_years}),'-',if(${ephemeral_months}&lt;10, concat('0',string(${ephemeral_months})), ${ephemeral_months}),'-',string(format-date-time(today(), "%d")))</t>
+    <t xml:space="preserve">concat(string(if(${ephemeral_months} &gt; 0,${ephemeral_years},${ephemeral_years} - 1)),'-',if(${ephemeral_months} &gt; 0,if(${ephemeral_months}&lt;10,concat('0',string(${ephemeral_months})),${ephemeral_months}),12),'-',string(format-date-time(today(), "%d")))</t>
   </si>
   <si>
     <t>dob_raw</t>
@@ -1151,7 +1151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <name val="Calibri"/>
@@ -1287,9 +1287,9 @@
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1756,12 +1756,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" workbookViewId="0" zoomScale="100">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="P39" activeCellId="0" sqref="P39"/>
     </sheetView>
   </sheetViews>
@@ -2682,7 +2682,7 @@
         <v>28</v>
       </c>
       <c r="J15" s="16"/>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L15" s="16" t="s">
@@ -2804,7 +2804,7 @@
       <c r="J17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L17" s="16"/>
@@ -3255,7 +3255,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="21" t="s">
+      <c r="R28" s="20" t="s">
         <v>107</v>
       </c>
       <c r="S28" s="16"/>
@@ -3494,7 +3494,7 @@
       <c r="B29" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="18"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -3548,7 +3548,7 @@
       <c r="B30" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -3603,20 +3603,20 @@
       <c r="C31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20" t="s">
+      <c r="H31" s="19"/>
+      <c r="I31" s="19" t="s">
         <v>28</v>
       </c>
       <c r="J31" s="16"/>
@@ -4069,7 +4069,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="16" t="s">
+      <c r="P39" s="21" t="s">
         <v>143</v>
       </c>
       <c r="Q39" s="16"/>
@@ -5997,7 +5997,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -6005,11 +6005,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6095,7 +6095,7 @@
         <v>231</v>
       </c>
       <c r="H2" s="30"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>232</v>
       </c>
       <c r="J2" s="8"/>
@@ -6139,7 +6139,7 @@
         <v>238</v>
       </c>
       <c r="H3" s="30"/>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>239</v>
       </c>
       <c r="J3" s="8"/>
@@ -6183,7 +6183,7 @@
         <v>246</v>
       </c>
       <c r="H4" s="30"/>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>247</v>
       </c>
       <c r="J4" s="8"/>
@@ -6227,7 +6227,7 @@
         <v>253</v>
       </c>
       <c r="H5" s="30"/>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>254</v>
       </c>
       <c r="J5" s="8"/>
@@ -6271,7 +6271,7 @@
         <v>260</v>
       </c>
       <c r="H6" s="30"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>261</v>
       </c>
       <c r="J6" s="8"/>
@@ -6315,7 +6315,7 @@
         <v>267</v>
       </c>
       <c r="H7" s="30"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>268</v>
       </c>
       <c r="J7" s="8"/>
@@ -6359,7 +6359,7 @@
         <v>274</v>
       </c>
       <c r="H8" s="30"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>275</v>
       </c>
       <c r="J8" s="8"/>
@@ -6395,7 +6395,7 @@
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -6437,7 +6437,7 @@
         <v>285</v>
       </c>
       <c r="H10" s="30"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>286</v>
       </c>
       <c r="J10" s="8"/>
@@ -6481,7 +6481,7 @@
         <v>292</v>
       </c>
       <c r="H11" s="30"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>293</v>
       </c>
       <c r="J11" s="8"/>
@@ -6525,7 +6525,7 @@
         <v>296</v>
       </c>
       <c r="H12" s="30"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>299</v>
       </c>
       <c r="J12" s="8"/>
@@ -6569,7 +6569,7 @@
         <v>305</v>
       </c>
       <c r="H13" s="30"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>306</v>
       </c>
       <c r="J13" s="8"/>
@@ -6613,7 +6613,7 @@
         <v>312</v>
       </c>
       <c r="H14" s="30"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>308</v>
       </c>
       <c r="J14" s="8"/>
@@ -6657,7 +6657,7 @@
         <v>315</v>
       </c>
       <c r="H15" s="30"/>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>318</v>
       </c>
       <c r="J15" s="8"/>
@@ -6701,7 +6701,7 @@
         <v>320</v>
       </c>
       <c r="H16" s="30"/>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>232</v>
       </c>
       <c r="J16" s="8"/>
@@ -6745,7 +6745,7 @@
         <v>325</v>
       </c>
       <c r="H17" s="30"/>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>326</v>
       </c>
       <c r="J17" s="8"/>
@@ -6789,7 +6789,7 @@
         <v>332</v>
       </c>
       <c r="H18" s="30"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>333</v>
       </c>
       <c r="J18" s="8"/>
@@ -6833,7 +6833,7 @@
         <v>339</v>
       </c>
       <c r="H19" s="30"/>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>340</v>
       </c>
       <c r="J19" s="8"/>
@@ -6877,7 +6877,7 @@
         <v>343</v>
       </c>
       <c r="H20" s="30"/>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>346</v>
       </c>
       <c r="J20" s="8"/>
@@ -6921,7 +6921,7 @@
         <v>351</v>
       </c>
       <c r="H21" s="30"/>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>352</v>
       </c>
       <c r="J21" s="8"/>
@@ -6965,7 +6965,7 @@
         <v>357</v>
       </c>
       <c r="H22" s="30"/>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>358</v>
       </c>
       <c r="J22" s="8"/>
@@ -7009,7 +7009,7 @@
         <v>363</v>
       </c>
       <c r="H23" s="30"/>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>364</v>
       </c>
       <c r="J23" s="8"/>
@@ -7053,7 +7053,7 @@
         <v>97</v>
       </c>
       <c r="H24" s="30"/>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
       <c r="J24" s="8"/>
@@ -7077,7 +7077,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -7085,11 +7085,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" workbookViewId="0" zoomScale="100">
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-03-11 17-37</v>
+        <v xml:space="preserve">2022-06-13 17-11</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>373</v>
@@ -13850,7 +13850,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add add-date XPath function
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
   <si>
     <t>type</t>
   </si>
@@ -428,25 +428,13 @@
     <t>horizontal</t>
   </si>
   <si>
-    <t>ephemeral_months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%m") - coalesce(../age_months, 0) + 12, format-date-time(today(),"%m") - coalesce(../age_months, 0))</t>
-  </si>
-  <si>
-    <t>ephemeral_years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
-  </si>
-  <si>
     <t>dob_approx</t>
   </si>
   <si>
     <t>DOB</t>
   </si>
   <si>
-    <t xml:space="preserve">concat(string(if(${ephemeral_months} &gt; 0,${ephemeral_years},${ephemeral_years} - 1)),'-',if(${ephemeral_months} &gt; 0,if(${ephemeral_months}&lt;10,concat('0',string(${ephemeral_months})),${ephemeral_months}),12),'-',string(format-date-time(today(), "%d")))</t>
+    <t xml:space="preserve">add-date(today(), 0-${age_years}, 0-${age_months})</t>
   </si>
   <si>
     <t>dob_raw</t>
@@ -466,9 +454,7 @@
     <t>dob_debug</t>
   </si>
   <si>
-    <t xml:space="preserve">Months: ${ephemeral_months}
-Year: ${ephemeral_years}
-DOB Approx: ${dob_approx}
+    <t xml:space="preserve">DOB Approx: ${dob_approx}
 DOB Calendar: ${dob_calendar}
 DOB ISO: ${dob_iso}</t>
   </si>
@@ -1261,7 +1247,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1290,6 +1276,9 @@
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3950,7 +3939,9 @@
       <c r="B37" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
@@ -3963,8 +3954,8 @@
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="16" t="s">
-        <v>138</v>
+      <c r="P37" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -4000,7 +3991,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="18"/>
@@ -4015,8 +4006,8 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="16" t="s">
-        <v>140</v>
+      <c r="P38" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
@@ -4052,10 +4043,10 @@
         <v>59</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="16"/>
@@ -4069,7 +4060,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="21" t="s">
+      <c r="P39" s="16" t="s">
         <v>143</v>
       </c>
       <c r="Q39" s="16"/>
@@ -4103,12 +4094,14 @@
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="23" t="s">
+        <v>145</v>
+      </c>
       <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
@@ -4116,14 +4109,15 @@
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
+      <c r="K40" s="16" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
-      <c r="P40" s="22" t="s">
-        <v>145</v>
-      </c>
+      <c r="P40" s="16"/>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
       <c r="S40" s="16"/>
@@ -4155,14 +4149,10 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>119</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -4175,9 +4165,7 @@
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
-      <c r="P41" s="16" t="s">
-        <v>147</v>
-      </c>
+      <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
@@ -4209,29 +4197,43 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="D42" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="E42" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>152</v>
+      </c>
       <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
+      <c r="I42" s="16" t="s">
+        <v>153</v>
+      </c>
       <c r="J42" s="16"/>
-      <c r="K42" s="16">
-        <f>FALSE()</f>
-        <v>0</v>
+      <c r="K42" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
+      <c r="N42" s="24" t="b">
+        <f t="shared" ref="N42:N43" si="0">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
@@ -4264,22 +4266,43 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+        <v>146</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
+      <c r="I43" s="16" t="s">
+        <v>161</v>
+      </c>
       <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
+      <c r="K43" s="16" t="s">
+        <v>92</v>
+      </c>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
+      <c r="N43" s="24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O43" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
@@ -4312,43 +4335,42 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="J44" s="16"/>
+        <v>168</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L44" s="16"/>
+      <c r="L44" s="16" t="s">
+        <v>136</v>
+      </c>
       <c r="M44" s="16"/>
-      <c r="N44" s="23">
-        <f t="shared" ref="N44:N45" si="0">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O44" s="16" t="s">
-        <v>158</v>
-      </c>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
@@ -4381,29 +4403,29 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="16" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="J45" s="16"/>
       <c r="K45" s="16" t="s">
@@ -4411,13 +4433,8 @@
       </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
-      <c r="N45" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O45" s="16" t="s">
-        <v>158</v>
-      </c>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
@@ -4450,39 +4467,37 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="17" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="16" t="s">
-        <v>136</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
@@ -4518,29 +4533,29 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="17" t="s">
-        <v>173</v>
+        <v>30</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16" t="s">
@@ -4585,34 +4600,34 @@
         <v>30</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J48" s="16"/>
       <c r="K48" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="L48" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
@@ -4648,35 +4663,25 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>194</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
       <c r="H49" s="16"/>
-      <c r="I49" s="16" t="s">
-        <v>195</v>
-      </c>
+      <c r="I49" s="16"/>
       <c r="J49" s="16"/>
-      <c r="K49" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
@@ -4712,41 +4717,27 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="F50" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="G50" s="16" t="s">
-        <v>200</v>
-      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
       <c r="H50" s="16"/>
-      <c r="I50" s="16" t="s">
-        <v>196</v>
-      </c>
+      <c r="I50" s="16"/>
       <c r="J50" s="16"/>
-      <c r="K50" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L50" s="16" t="s">
-        <v>201</v>
-      </c>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="16"/>
+      <c r="P50" s="16" t="s">
+        <v>200</v>
+      </c>
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
       <c r="S50" s="16"/>
@@ -4778,14 +4769,12 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>28</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
       <c r="F51" s="16"/>
@@ -4794,13 +4783,13 @@
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
       <c r="K51" s="16"/>
-      <c r="L51" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
-      <c r="P51" s="16"/>
+      <c r="P51" s="16" t="s">
+        <v>202</v>
+      </c>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
       <c r="S51" s="16"/>
@@ -4884,11 +4873,9 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>205</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B53" s="17"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -4902,9 +4889,7 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="P53" s="16"/>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
       <c r="S53" s="16"/>
@@ -4936,11 +4921,9 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>207</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B54" s="17"/>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -4954,9 +4937,7 @@
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
-      <c r="P54" s="16" t="s">
-        <v>208</v>
-      </c>
+      <c r="P54" s="16"/>
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
       <c r="S54" s="16"/>
@@ -4987,68 +4968,76 @@
       <c r="AR54" s="16"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="15"/>
       <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="16"/>
-      <c r="O55" s="16"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
-      <c r="S55" s="16"/>
-      <c r="T55" s="16"/>
-      <c r="U55" s="16"/>
-      <c r="V55" s="16"/>
-      <c r="W55" s="16"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="15"/>
       <c r="X55" s="16"/>
-      <c r="Y55" s="16"/>
-      <c r="Z55" s="16"/>
-      <c r="AA55" s="16"/>
-      <c r="AB55" s="16"/>
-      <c r="AC55" s="16"/>
-      <c r="AD55" s="16"/>
-      <c r="AE55" s="16"/>
-      <c r="AF55" s="16"/>
-      <c r="AG55" s="16"/>
-      <c r="AH55" s="16"/>
-      <c r="AI55" s="16"/>
-      <c r="AJ55" s="16"/>
-      <c r="AK55" s="16"/>
-      <c r="AL55" s="16"/>
-      <c r="AM55" s="16"/>
-      <c r="AN55" s="16"/>
-      <c r="AO55" s="16"/>
-      <c r="AP55" s="16"/>
-      <c r="AQ55" s="16"/>
-      <c r="AR55" s="16"/>
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="8"/>
+      <c r="AB55" s="8"/>
+      <c r="AC55" s="8"/>
+      <c r="AD55" s="8"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="8"/>
+      <c r="AG55" s="8"/>
+      <c r="AH55" s="8"/>
+      <c r="AI55" s="8"/>
+      <c r="AJ55" s="8"/>
+      <c r="AK55" s="8"/>
+      <c r="AL55" s="8"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
+      <c r="I56" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J56" s="16"/>
       <c r="K56" s="16"/>
-      <c r="L56" s="16"/>
+      <c r="L56" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
       <c r="O56" s="16"/>
@@ -5083,51 +5072,75 @@
       <c r="AR56" s="16"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="8"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="12"/>
-      <c r="U57" s="13"/>
-      <c r="V57" s="14"/>
-      <c r="W57" s="15"/>
+      <c r="A57" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+      <c r="T57" s="16"/>
+      <c r="U57" s="16"/>
+      <c r="V57" s="16"/>
+      <c r="W57" s="16"/>
       <c r="X57" s="16"/>
-      <c r="Y57" s="8"/>
-      <c r="Z57" s="8"/>
-      <c r="AA57" s="8"/>
-      <c r="AB57" s="8"/>
-      <c r="AC57" s="8"/>
-      <c r="AD57" s="8"/>
-      <c r="AE57" s="8"/>
-      <c r="AF57" s="8"/>
-      <c r="AG57" s="8"/>
-      <c r="AH57" s="8"/>
-      <c r="AI57" s="8"/>
-      <c r="AJ57" s="8"/>
-      <c r="AK57" s="8"/>
-      <c r="AL57" s="8"/>
+      <c r="Y57" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z57" s="16"/>
+      <c r="AA57" s="16"/>
+      <c r="AB57" s="16"/>
+      <c r="AC57" s="16"/>
+      <c r="AD57" s="16"/>
+      <c r="AE57" s="16"/>
+      <c r="AF57" s="16"/>
+      <c r="AG57" s="16"/>
+      <c r="AH57" s="16"/>
+      <c r="AI57" s="16"/>
+      <c r="AJ57" s="16"/>
+      <c r="AK57" s="16"/>
+      <c r="AL57" s="16"/>
+      <c r="AM57" s="16"/>
+      <c r="AN57" s="16"/>
+      <c r="AO57" s="16"/>
+      <c r="AP57" s="16"/>
+      <c r="AQ57" s="16"/>
+      <c r="AR57" s="16"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="17" t="s">
-        <v>26</v>
+      <c r="A58" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>28</v>
@@ -5150,9 +5163,7 @@
       </c>
       <c r="J58" s="16"/>
       <c r="K58" s="16"/>
-      <c r="L58" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="L58" s="16"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
       <c r="O58" s="16"/>
@@ -5187,34 +5198,40 @@
       <c r="AR58" s="16"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="24" t="s">
-        <v>58</v>
+      <c r="A59" s="17" t="s">
+        <v>205</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>28</v>
+        <v>209</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>28</v>
+        <v>211</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="16"/>
+        <v>212</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K59" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
@@ -5228,7 +5245,7 @@
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
       <c r="Y59" s="16" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
       <c r="Z59" s="16"/>
       <c r="AA59" s="16"/>
@@ -5251,38 +5268,42 @@
       <c r="AR59" s="16"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="24" t="s">
-        <v>58</v>
+      <c r="A60" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>28</v>
+        <v>215</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J60" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="J60" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K60" s="16"/>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="16"/>
@@ -5314,39 +5335,33 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>209</v>
+        <v>30</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="J61" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K61" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="L61" s="16" t="s">
-        <v>48</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
       <c r="O61" s="16"/>
@@ -5359,9 +5374,7 @@
       <c r="V61" s="16"/>
       <c r="W61" s="16"/>
       <c r="X61" s="16"/>
-      <c r="Y61" s="16" t="s">
-        <v>218</v>
-      </c>
+      <c r="Y61" s="16"/>
       <c r="Z61" s="16"/>
       <c r="AA61" s="16"/>
       <c r="AB61" s="16"/>
@@ -5384,41 +5397,39 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>97</v>
+        <v>192</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>97</v>
+        <v>195</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J62" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J62" s="16"/>
       <c r="K62" s="16"/>
-      <c r="L62" s="16"/>
+      <c r="L62" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="16" t="s">
-        <v>220</v>
-      </c>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
       <c r="Q62" s="16"/>
       <c r="R62" s="16"/>
       <c r="S62" s="16"/>
@@ -5450,37 +5461,27 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D63" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>194</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
       <c r="H63" s="16"/>
-      <c r="I63" s="16" t="s">
-        <v>195</v>
-      </c>
+      <c r="I63" s="16"/>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
       <c r="O63" s="16"/>
-      <c r="P63" s="16"/>
+      <c r="P63" s="16" t="s">
+        <v>218</v>
+      </c>
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
       <c r="S63" s="16"/>
@@ -5512,39 +5513,27 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>200</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
       <c r="H64" s="16"/>
-      <c r="I64" s="16" t="s">
-        <v>196</v>
-      </c>
+      <c r="I64" s="16"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
-      <c r="L64" s="16" t="s">
-        <v>201</v>
-      </c>
+      <c r="L64" s="16"/>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
-      <c r="P64" s="16"/>
+      <c r="P64" s="16" t="s">
+        <v>220</v>
+      </c>
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="16"/>
@@ -5576,27 +5565,39 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
+        <v>198</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
+      <c r="I65" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
+      <c r="L65" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
       <c r="O65" s="16"/>
-      <c r="P65" s="16" t="s">
-        <v>222</v>
-      </c>
+      <c r="P65" s="16"/>
       <c r="Q65" s="16"/>
       <c r="R65" s="16"/>
       <c r="S65" s="16"/>
@@ -5631,7 +5632,7 @@
         <v>59</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
@@ -5647,7 +5648,7 @@
       <c r="N66" s="16"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
@@ -5680,39 +5681,27 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>28</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
       <c r="H67" s="16"/>
-      <c r="I67" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I67" s="16"/>
       <c r="J67" s="16"/>
       <c r="K67" s="16"/>
-      <c r="L67" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L67" s="16"/>
       <c r="M67" s="16"/>
       <c r="N67" s="16"/>
       <c r="O67" s="16"/>
-      <c r="P67" s="16"/>
+      <c r="P67" s="16" t="s">
+        <v>202</v>
+      </c>
       <c r="Q67" s="16"/>
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
@@ -5796,11 +5785,9 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>205</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B69" s="17"/>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
@@ -5814,9 +5801,7 @@
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
-      <c r="P69" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="P69" s="16"/>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
@@ -5848,11 +5833,9 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>207</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B70" s="17"/>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
@@ -5866,9 +5849,7 @@
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
       <c r="O70" s="16"/>
-      <c r="P70" s="16" t="s">
-        <v>208</v>
-      </c>
+      <c r="P70" s="16"/>
       <c r="Q70" s="16"/>
       <c r="R70" s="16"/>
       <c r="S70" s="16"/>
@@ -5897,102 +5878,6 @@
       <c r="AP70" s="16"/>
       <c r="AQ70" s="16"/>
       <c r="AR70" s="16"/>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
-      <c r="M71" s="16"/>
-      <c r="N71" s="16"/>
-      <c r="O71" s="16"/>
-      <c r="P71" s="16"/>
-      <c r="Q71" s="16"/>
-      <c r="R71" s="16"/>
-      <c r="S71" s="16"/>
-      <c r="T71" s="16"/>
-      <c r="U71" s="16"/>
-      <c r="V71" s="16"/>
-      <c r="W71" s="16"/>
-      <c r="X71" s="16"/>
-      <c r="Y71" s="16"/>
-      <c r="Z71" s="16"/>
-      <c r="AA71" s="16"/>
-      <c r="AB71" s="16"/>
-      <c r="AC71" s="16"/>
-      <c r="AD71" s="16"/>
-      <c r="AE71" s="16"/>
-      <c r="AF71" s="16"/>
-      <c r="AG71" s="16"/>
-      <c r="AH71" s="16"/>
-      <c r="AI71" s="16"/>
-      <c r="AJ71" s="16"/>
-      <c r="AK71" s="16"/>
-      <c r="AL71" s="16"/>
-      <c r="AM71" s="16"/>
-      <c r="AN71" s="16"/>
-      <c r="AO71" s="16"/>
-      <c r="AP71" s="16"/>
-      <c r="AQ71" s="16"/>
-      <c r="AR71" s="16"/>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B72" s="17"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="16"/>
-      <c r="J72" s="16"/>
-      <c r="K72" s="16"/>
-      <c r="L72" s="16"/>
-      <c r="M72" s="16"/>
-      <c r="N72" s="16"/>
-      <c r="O72" s="16"/>
-      <c r="P72" s="16"/>
-      <c r="Q72" s="16"/>
-      <c r="R72" s="16"/>
-      <c r="S72" s="16"/>
-      <c r="T72" s="16"/>
-      <c r="U72" s="16"/>
-      <c r="V72" s="16"/>
-      <c r="W72" s="16"/>
-      <c r="X72" s="16"/>
-      <c r="Y72" s="16"/>
-      <c r="Z72" s="16"/>
-      <c r="AA72" s="16"/>
-      <c r="AB72" s="16"/>
-      <c r="AC72" s="16"/>
-      <c r="AD72" s="16"/>
-      <c r="AE72" s="16"/>
-      <c r="AF72" s="16"/>
-      <c r="AG72" s="16"/>
-      <c r="AH72" s="16"/>
-      <c r="AI72" s="16"/>
-      <c r="AJ72" s="16"/>
-      <c r="AK72" s="16"/>
-      <c r="AL72" s="16"/>
-      <c r="AM72" s="16"/>
-      <c r="AN72" s="16"/>
-      <c r="AO72" s="16"/>
-      <c r="AP72" s="16"/>
-      <c r="AQ72" s="16"/>
-      <c r="AR72" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -6027,13 +5912,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -6073,30 +5958,30 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="G2" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -6117,30 +6002,30 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="G3" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="19" t="s">
         <v>235</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="19" t="s">
-        <v>239</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6161,30 +6046,30 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="F4" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="G4" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="H4" s="31"/>
+      <c r="I4" s="19" t="s">
         <v>243</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="19" t="s">
-        <v>247</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -6205,30 +6090,30 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="G5" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="H5" s="31"/>
+      <c r="I5" s="19" t="s">
         <v>250</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="19" t="s">
-        <v>254</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -6249,30 +6134,30 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="G6" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="H6" s="31"/>
+      <c r="I6" s="19" t="s">
         <v>257</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>260</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="19" t="s">
-        <v>261</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -6293,30 +6178,30 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="G7" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="H7" s="31"/>
+      <c r="I7" s="19" t="s">
         <v>264</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>266</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="19" t="s">
-        <v>268</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -6337,30 +6222,30 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="G8" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="19" t="s">
         <v>271</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>273</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="19" t="s">
-        <v>275</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -6382,19 +6267,19 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>278</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+        <v>272</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -6416,29 +6301,29 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="F10" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="G10" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="H10" s="31"/>
+      <c r="I10" s="19" t="s">
         <v>282</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="19" t="s">
-        <v>286</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -6460,29 +6345,29 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B11" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="G11" s="30" t="s">
         <v>288</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="H11" s="31"/>
+      <c r="I11" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>291</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="19" t="s">
-        <v>293</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -6504,29 +6389,29 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="F12" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="G12" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>296</v>
-      </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="19" t="s">
-        <v>299</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6548,29 +6433,29 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B13" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="G13" s="30" t="s">
         <v>301</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="H13" s="31"/>
+      <c r="I13" s="19" t="s">
         <v>302</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="19" t="s">
-        <v>306</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -6592,29 +6477,29 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="F14" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="G14" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>311</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="19" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -6636,29 +6521,29 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B15" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="F15" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="G15" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="H15" s="31"/>
+      <c r="I15" s="19" t="s">
         <v>314</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="19" t="s">
-        <v>318</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -6679,30 +6564,30 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="D16" s="27" t="s">
+      <c r="A16" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="H16" s="31"/>
+      <c r="I16" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -6723,30 +6608,30 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="E17" s="33" t="s">
         <v>319</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="F17" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="G17" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="H17" s="31"/>
+      <c r="I17" s="19" t="s">
         <v>322</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>324</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>325</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="19" t="s">
-        <v>326</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -6770,27 +6655,27 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="F18" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="G18" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="H18" s="31"/>
+      <c r="I18" s="19" t="s">
         <v>329</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>330</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="19" t="s">
-        <v>333</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6814,27 +6699,27 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="G19" s="30" t="s">
         <v>335</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="H19" s="31"/>
+      <c r="I19" s="19" t="s">
         <v>336</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>338</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="19" t="s">
-        <v>340</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6858,27 +6743,27 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="G20" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="19" t="s">
         <v>342</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>344</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="19" t="s">
-        <v>346</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6902,27 +6787,27 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>327</v>
-      </c>
-      <c r="C21" s="34" t="s">
+      <c r="B21" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="G21" s="30" t="s">
         <v>347</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="H21" s="31"/>
+      <c r="I21" s="19" t="s">
         <v>348</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>349</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>350</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>351</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="19" t="s">
-        <v>352</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6946,27 +6831,27 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="C22" s="34" t="s">
+      <c r="B22" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>349</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="G22" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="H22" s="31"/>
+      <c r="I22" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>355</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>356</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>357</v>
-      </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="19" t="s">
-        <v>358</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -6990,27 +6875,27 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="G23" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="H23" s="31"/>
+      <c r="I23" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>363</v>
-      </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="19" t="s">
-        <v>364</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -7031,28 +6916,28 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="36" t="s">
-        <v>365</v>
-      </c>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
@@ -7108,19 +6993,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7145,20 +7030,20 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="C2" s="37" t="str">
+        <v>368</v>
+      </c>
+      <c r="C2" s="38" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-06-13 17-11</v>
+        <v xml:space="preserve">2022-08-15 11-54</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>

</xml_diff>

<commit_message>
Update default contact forms to use `columns` appearance
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -161,7 +161,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>horizontal-compact</t>
+    <t>columns-pack</t>
   </si>
   <si>
     <t>db:person</t>
@@ -425,7 +425,7 @@
     <t>DELETE_THIS_LINE</t>
   </si>
   <si>
-    <t>horizontal</t>
+    <t>columns</t>
   </si>
   <si>
     <t>ephemeral_months</t>
@@ -1284,12 +1284,12 @@
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2435,7 +2435,7 @@
         <v>47</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="18" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="16"/>
@@ -2623,7 +2623,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="18" t="s">
+      <c r="P14" s="19" t="s">
         <v>61</v>
       </c>
       <c r="Q14" s="16"/>
@@ -2665,7 +2665,7 @@
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -2731,7 +2731,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="18"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2742,8 +2742,8 @@
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18" t="s">
+      <c r="O16" s="19"/>
+      <c r="P16" s="19" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="16"/>
@@ -2877,7 +2877,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="18"/>
+      <c r="P18" s="19"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
@@ -2886,7 +2886,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
-      <c r="Y18" s="18" t="s">
+      <c r="Y18" s="19" t="s">
         <v>79</v>
       </c>
       <c r="Z18" s="16"/>
@@ -2929,7 +2929,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="18" t="s">
+      <c r="P19" s="19" t="s">
         <v>81</v>
       </c>
       <c r="Q19" s="16"/>
@@ -3004,7 +3004,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="18" t="s">
+      <c r="Y20" s="19" t="s">
         <v>79</v>
       </c>
       <c r="Z20" s="16"/>
@@ -3047,7 +3047,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="18" t="s">
+      <c r="P21" s="19" t="s">
         <v>85</v>
       </c>
       <c r="Q21" s="16"/>
@@ -3255,7 +3255,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="19"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="C27" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -3457,7 +3457,7 @@
       </c>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="20" t="s">
+      <c r="R28" s="21" t="s">
         <v>107</v>
       </c>
       <c r="S28" s="16"/>
@@ -3494,8 +3494,8 @@
       <c r="B29" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -3548,8 +3548,8 @@
       <c r="B30" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3603,20 +3603,20 @@
       <c r="C31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19" t="s">
+      <c r="H31" s="20"/>
+      <c r="I31" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J31" s="16"/>
@@ -3665,7 +3665,7 @@
       <c r="C32" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -3781,7 +3781,7 @@
       <c r="C34" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -3841,7 +3841,7 @@
       <c r="C35" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="18"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -3899,7 +3899,7 @@
       <c r="C36" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="18"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -3907,7 +3907,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="16" t="s">
+      <c r="L36" s="18" t="s">
         <v>136</v>
       </c>
       <c r="M36" s="16"/>
@@ -3951,7 +3951,7 @@
         <v>137</v>
       </c>
       <c r="C37" s="16"/>
-      <c r="D37" s="18"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -4003,7 +4003,7 @@
         <v>139</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="18"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -4057,7 +4057,7 @@
       <c r="C39" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="D39" s="18"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -4069,7 +4069,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="21" t="s">
+      <c r="P39" s="16" t="s">
         <v>143</v>
       </c>
       <c r="Q39" s="16"/>
@@ -4109,7 +4109,7 @@
         <v>144</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="18"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
@@ -4163,7 +4163,7 @@
       <c r="C41" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="18"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -4217,7 +4217,7 @@
       <c r="C42" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="18"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
@@ -4268,7 +4268,7 @@
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="16"/>
-      <c r="D43" s="18"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
@@ -4480,7 +4480,7 @@
       <c r="K46" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L46" s="16" t="s">
+      <c r="L46" s="18" t="s">
         <v>136</v>
       </c>
       <c r="M46" s="16"/>
@@ -5344,7 +5344,7 @@
       <c r="K61" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="L61" s="16" t="s">
+      <c r="L61" s="18" t="s">
         <v>48</v>
       </c>
       <c r="M61" s="16"/>
@@ -5392,7 +5392,7 @@
       <c r="C62" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="19" t="s">
         <v>97</v>
       </c>
       <c r="E62" s="16" t="s">
@@ -5467,7 +5467,7 @@
       <c r="F63" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="G63" s="18" t="s">
+      <c r="G63" s="19" t="s">
         <v>194</v>
       </c>
       <c r="H63" s="16"/>
@@ -5529,7 +5529,7 @@
       <c r="F64" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="G64" s="18" t="s">
+      <c r="G64" s="19" t="s">
         <v>200</v>
       </c>
       <c r="H64" s="16"/>
@@ -5697,7 +5697,7 @@
       <c r="F67" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G67" s="18" t="s">
+      <c r="G67" s="19" t="s">
         <v>28</v>
       </c>
       <c r="H67" s="16"/>
@@ -6095,7 +6095,7 @@
         <v>231</v>
       </c>
       <c r="H2" s="30"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="20" t="s">
         <v>232</v>
       </c>
       <c r="J2" s="8"/>
@@ -6139,7 +6139,7 @@
         <v>238</v>
       </c>
       <c r="H3" s="30"/>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="20" t="s">
         <v>239</v>
       </c>
       <c r="J3" s="8"/>
@@ -6183,7 +6183,7 @@
         <v>246</v>
       </c>
       <c r="H4" s="30"/>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="20" t="s">
         <v>247</v>
       </c>
       <c r="J4" s="8"/>
@@ -6227,7 +6227,7 @@
         <v>253</v>
       </c>
       <c r="H5" s="30"/>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="20" t="s">
         <v>254</v>
       </c>
       <c r="J5" s="8"/>
@@ -6271,7 +6271,7 @@
         <v>260</v>
       </c>
       <c r="H6" s="30"/>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="20" t="s">
         <v>261</v>
       </c>
       <c r="J6" s="8"/>
@@ -6315,7 +6315,7 @@
         <v>267</v>
       </c>
       <c r="H7" s="30"/>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="20" t="s">
         <v>268</v>
       </c>
       <c r="J7" s="8"/>
@@ -6359,7 +6359,7 @@
         <v>274</v>
       </c>
       <c r="H8" s="30"/>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="20" t="s">
         <v>275</v>
       </c>
       <c r="J8" s="8"/>
@@ -6395,7 +6395,7 @@
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -6437,7 +6437,7 @@
         <v>285</v>
       </c>
       <c r="H10" s="30"/>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="20" t="s">
         <v>286</v>
       </c>
       <c r="J10" s="8"/>
@@ -6481,7 +6481,7 @@
         <v>292</v>
       </c>
       <c r="H11" s="30"/>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="20" t="s">
         <v>293</v>
       </c>
       <c r="J11" s="8"/>
@@ -6525,7 +6525,7 @@
         <v>296</v>
       </c>
       <c r="H12" s="30"/>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="20" t="s">
         <v>299</v>
       </c>
       <c r="J12" s="8"/>
@@ -6569,7 +6569,7 @@
         <v>305</v>
       </c>
       <c r="H13" s="30"/>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="20" t="s">
         <v>306</v>
       </c>
       <c r="J13" s="8"/>
@@ -6613,7 +6613,7 @@
         <v>312</v>
       </c>
       <c r="H14" s="30"/>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="20" t="s">
         <v>308</v>
       </c>
       <c r="J14" s="8"/>
@@ -6657,7 +6657,7 @@
         <v>315</v>
       </c>
       <c r="H15" s="30"/>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="20" t="s">
         <v>318</v>
       </c>
       <c r="J15" s="8"/>
@@ -6701,7 +6701,7 @@
         <v>320</v>
       </c>
       <c r="H16" s="30"/>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="20" t="s">
         <v>232</v>
       </c>
       <c r="J16" s="8"/>
@@ -6745,7 +6745,7 @@
         <v>325</v>
       </c>
       <c r="H17" s="30"/>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>326</v>
       </c>
       <c r="J17" s="8"/>
@@ -6789,7 +6789,7 @@
         <v>332</v>
       </c>
       <c r="H18" s="30"/>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="20" t="s">
         <v>333</v>
       </c>
       <c r="J18" s="8"/>
@@ -6833,7 +6833,7 @@
         <v>339</v>
       </c>
       <c r="H19" s="30"/>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="20" t="s">
         <v>340</v>
       </c>
       <c r="J19" s="8"/>
@@ -6877,7 +6877,7 @@
         <v>343</v>
       </c>
       <c r="H20" s="30"/>
-      <c r="I20" s="19" t="s">
+      <c r="I20" s="20" t="s">
         <v>346</v>
       </c>
       <c r="J20" s="8"/>
@@ -6921,7 +6921,7 @@
         <v>351</v>
       </c>
       <c r="H21" s="30"/>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="20" t="s">
         <v>352</v>
       </c>
       <c r="J21" s="8"/>
@@ -6965,7 +6965,7 @@
         <v>357</v>
       </c>
       <c r="H22" s="30"/>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="20" t="s">
         <v>358</v>
       </c>
       <c r="J22" s="8"/>
@@ -7009,7 +7009,7 @@
         <v>363</v>
       </c>
       <c r="H23" s="30"/>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="20" t="s">
         <v>364</v>
       </c>
       <c r="J23" s="8"/>
@@ -7053,7 +7053,7 @@
         <v>97</v>
       </c>
       <c r="H24" s="30"/>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="20" t="s">
         <v>100</v>
       </c>
       <c r="J24" s="8"/>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-06-13 17-11</v>
+        <v xml:space="preserve">2022-08-19 14-44</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>373</v>

</xml_diff>

<commit_message>
7694 - Add `add-date` XPath function (#7729)
(cherry picked from commit cde05fc7774e2cd2dbeefe6f3fea97c8529cae4c)
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
   <si>
     <t>type</t>
   </si>
@@ -428,25 +428,13 @@
     <t>horizontal</t>
   </si>
   <si>
-    <t>ephemeral_months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%m") - coalesce(../age_months, 0) + 12, format-date-time(today(),"%m") - coalesce(../age_months, 0))</t>
-  </si>
-  <si>
-    <t>ephemeral_years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(format-date-time(today(),"%m") - coalesce(../age_months, 0) &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
-  </si>
-  <si>
     <t>dob_approx</t>
   </si>
   <si>
     <t>DOB</t>
   </si>
   <si>
-    <t xml:space="preserve">concat(string(if(${ephemeral_months} &gt; 0,${ephemeral_years},${ephemeral_years} - 1)),'-',if(${ephemeral_months} &gt; 0,if(${ephemeral_months}&lt;10,concat('0',string(${ephemeral_months})),${ephemeral_months}),12),'-',string(format-date-time(today(), "%d")))</t>
+    <t xml:space="preserve">add-date(today(), 0-${age_years}, 0-${age_months})</t>
   </si>
   <si>
     <t>dob_raw</t>
@@ -466,9 +454,7 @@
     <t>dob_debug</t>
   </si>
   <si>
-    <t xml:space="preserve">Months: ${ephemeral_months}
-Year: ${ephemeral_years}
-DOB Approx: ${dob_approx}
+    <t xml:space="preserve">DOB Approx: ${dob_approx}
 DOB Calendar: ${dob_calendar}
 DOB ISO: ${dob_iso}</t>
   </si>
@@ -1261,7 +1247,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1290,6 +1276,9 @@
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3950,7 +3939,9 @@
       <c r="B37" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
@@ -3963,8 +3954,8 @@
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="16" t="s">
-        <v>138</v>
+      <c r="P37" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -4000,7 +3991,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="18"/>
@@ -4015,8 +4006,8 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="16" t="s">
-        <v>140</v>
+      <c r="P38" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
@@ -4052,10 +4043,10 @@
         <v>59</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="16"/>
@@ -4069,7 +4060,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
-      <c r="P39" s="21" t="s">
+      <c r="P39" s="16" t="s">
         <v>143</v>
       </c>
       <c r="Q39" s="16"/>
@@ -4103,12 +4094,14 @@
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="23" t="s">
+        <v>145</v>
+      </c>
       <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
@@ -4116,14 +4109,15 @@
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
+      <c r="K40" s="16" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
-      <c r="P40" s="22" t="s">
-        <v>145</v>
-      </c>
+      <c r="P40" s="16"/>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
       <c r="S40" s="16"/>
@@ -4155,14 +4149,10 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>119</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -4175,9 +4165,7 @@
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
-      <c r="P41" s="16" t="s">
-        <v>147</v>
-      </c>
+      <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
@@ -4209,29 +4197,43 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="D42" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="E42" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>152</v>
+      </c>
       <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
+      <c r="I42" s="16" t="s">
+        <v>153</v>
+      </c>
       <c r="J42" s="16"/>
-      <c r="K42" s="16">
-        <f>FALSE()</f>
-        <v>0</v>
+      <c r="K42" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
+      <c r="N42" s="24" t="b">
+        <f t="shared" ref="N42:N43" si="0">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O42" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
@@ -4264,22 +4266,43 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+        <v>146</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
+      <c r="I43" s="16" t="s">
+        <v>161</v>
+      </c>
       <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
+      <c r="K43" s="16" t="s">
+        <v>92</v>
+      </c>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
+      <c r="N43" s="24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O43" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
@@ -4312,43 +4335,42 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="J44" s="16"/>
+        <v>168</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L44" s="16"/>
+      <c r="L44" s="16" t="s">
+        <v>136</v>
+      </c>
       <c r="M44" s="16"/>
-      <c r="N44" s="23">
-        <f t="shared" ref="N44:N45" si="0">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O44" s="16" t="s">
-        <v>158</v>
-      </c>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
@@ -4381,29 +4403,29 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="16" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="J45" s="16"/>
       <c r="K45" s="16" t="s">
@@ -4411,13 +4433,8 @@
       </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
-      <c r="N45" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O45" s="16" t="s">
-        <v>158</v>
-      </c>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
@@ -4450,39 +4467,37 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="17" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="16" t="s">
-        <v>136</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
@@ -4518,29 +4533,29 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="17" t="s">
-        <v>173</v>
+        <v>30</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16" t="s">
@@ -4585,34 +4600,34 @@
         <v>30</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="J48" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J48" s="16"/>
       <c r="K48" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="L48" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
@@ -4648,35 +4663,25 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>194</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
       <c r="H49" s="16"/>
-      <c r="I49" s="16" t="s">
-        <v>195</v>
-      </c>
+      <c r="I49" s="16"/>
       <c r="J49" s="16"/>
-      <c r="K49" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
@@ -4712,41 +4717,27 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="F50" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="G50" s="16" t="s">
-        <v>200</v>
-      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
       <c r="H50" s="16"/>
-      <c r="I50" s="16" t="s">
-        <v>196</v>
-      </c>
+      <c r="I50" s="16"/>
       <c r="J50" s="16"/>
-      <c r="K50" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L50" s="16" t="s">
-        <v>201</v>
-      </c>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="16"/>
+      <c r="P50" s="16" t="s">
+        <v>200</v>
+      </c>
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
       <c r="S50" s="16"/>
@@ -4778,14 +4769,12 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>28</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
       <c r="F51" s="16"/>
@@ -4794,13 +4783,13 @@
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
       <c r="K51" s="16"/>
-      <c r="L51" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
-      <c r="P51" s="16"/>
+      <c r="P51" s="16" t="s">
+        <v>202</v>
+      </c>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
       <c r="S51" s="16"/>
@@ -4884,11 +4873,9 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>205</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B53" s="17"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -4902,9 +4889,7 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="P53" s="16"/>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
       <c r="S53" s="16"/>
@@ -4936,11 +4921,9 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>207</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B54" s="17"/>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -4954,9 +4937,7 @@
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
-      <c r="P54" s="16" t="s">
-        <v>208</v>
-      </c>
+      <c r="P54" s="16"/>
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
       <c r="S54" s="16"/>
@@ -4987,68 +4968,76 @@
       <c r="AR54" s="16"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="15"/>
       <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="16"/>
-      <c r="O55" s="16"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
-      <c r="S55" s="16"/>
-      <c r="T55" s="16"/>
-      <c r="U55" s="16"/>
-      <c r="V55" s="16"/>
-      <c r="W55" s="16"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="13"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="15"/>
       <c r="X55" s="16"/>
-      <c r="Y55" s="16"/>
-      <c r="Z55" s="16"/>
-      <c r="AA55" s="16"/>
-      <c r="AB55" s="16"/>
-      <c r="AC55" s="16"/>
-      <c r="AD55" s="16"/>
-      <c r="AE55" s="16"/>
-      <c r="AF55" s="16"/>
-      <c r="AG55" s="16"/>
-      <c r="AH55" s="16"/>
-      <c r="AI55" s="16"/>
-      <c r="AJ55" s="16"/>
-      <c r="AK55" s="16"/>
-      <c r="AL55" s="16"/>
-      <c r="AM55" s="16"/>
-      <c r="AN55" s="16"/>
-      <c r="AO55" s="16"/>
-      <c r="AP55" s="16"/>
-      <c r="AQ55" s="16"/>
-      <c r="AR55" s="16"/>
+      <c r="Y55" s="8"/>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="8"/>
+      <c r="AB55" s="8"/>
+      <c r="AC55" s="8"/>
+      <c r="AD55" s="8"/>
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="8"/>
+      <c r="AG55" s="8"/>
+      <c r="AH55" s="8"/>
+      <c r="AI55" s="8"/>
+      <c r="AJ55" s="8"/>
+      <c r="AK55" s="8"/>
+      <c r="AL55" s="8"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
+      <c r="I56" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J56" s="16"/>
       <c r="K56" s="16"/>
-      <c r="L56" s="16"/>
+      <c r="L56" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
       <c r="O56" s="16"/>
@@ -5083,51 +5072,75 @@
       <c r="AR56" s="16"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
-      <c r="Q57" s="8"/>
-      <c r="R57" s="8"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="12"/>
-      <c r="U57" s="13"/>
-      <c r="V57" s="14"/>
-      <c r="W57" s="15"/>
+      <c r="A57" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+      <c r="T57" s="16"/>
+      <c r="U57" s="16"/>
+      <c r="V57" s="16"/>
+      <c r="W57" s="16"/>
       <c r="X57" s="16"/>
-      <c r="Y57" s="8"/>
-      <c r="Z57" s="8"/>
-      <c r="AA57" s="8"/>
-      <c r="AB57" s="8"/>
-      <c r="AC57" s="8"/>
-      <c r="AD57" s="8"/>
-      <c r="AE57" s="8"/>
-      <c r="AF57" s="8"/>
-      <c r="AG57" s="8"/>
-      <c r="AH57" s="8"/>
-      <c r="AI57" s="8"/>
-      <c r="AJ57" s="8"/>
-      <c r="AK57" s="8"/>
-      <c r="AL57" s="8"/>
+      <c r="Y57" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z57" s="16"/>
+      <c r="AA57" s="16"/>
+      <c r="AB57" s="16"/>
+      <c r="AC57" s="16"/>
+      <c r="AD57" s="16"/>
+      <c r="AE57" s="16"/>
+      <c r="AF57" s="16"/>
+      <c r="AG57" s="16"/>
+      <c r="AH57" s="16"/>
+      <c r="AI57" s="16"/>
+      <c r="AJ57" s="16"/>
+      <c r="AK57" s="16"/>
+      <c r="AL57" s="16"/>
+      <c r="AM57" s="16"/>
+      <c r="AN57" s="16"/>
+      <c r="AO57" s="16"/>
+      <c r="AP57" s="16"/>
+      <c r="AQ57" s="16"/>
+      <c r="AR57" s="16"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="17" t="s">
-        <v>26</v>
+      <c r="A58" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>28</v>
@@ -5150,9 +5163,7 @@
       </c>
       <c r="J58" s="16"/>
       <c r="K58" s="16"/>
-      <c r="L58" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="L58" s="16"/>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
       <c r="O58" s="16"/>
@@ -5187,34 +5198,40 @@
       <c r="AR58" s="16"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="24" t="s">
-        <v>58</v>
+      <c r="A59" s="17" t="s">
+        <v>205</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>28</v>
+        <v>209</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>28</v>
+        <v>211</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="16"/>
+        <v>212</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K59" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="L59" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
@@ -5228,7 +5245,7 @@
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
       <c r="Y59" s="16" t="s">
-        <v>94</v>
+        <v>214</v>
       </c>
       <c r="Z59" s="16"/>
       <c r="AA59" s="16"/>
@@ -5251,38 +5268,42 @@
       <c r="AR59" s="16"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="24" t="s">
-        <v>58</v>
+      <c r="A60" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>28</v>
+        <v>215</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J60" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="J60" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K60" s="16"/>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="16"/>
@@ -5314,39 +5335,33 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>209</v>
+        <v>30</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="J61" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K61" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="L61" s="16" t="s">
-        <v>48</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
       <c r="O61" s="16"/>
@@ -5359,9 +5374,7 @@
       <c r="V61" s="16"/>
       <c r="W61" s="16"/>
       <c r="X61" s="16"/>
-      <c r="Y61" s="16" t="s">
-        <v>218</v>
-      </c>
+      <c r="Y61" s="16"/>
       <c r="Z61" s="16"/>
       <c r="AA61" s="16"/>
       <c r="AB61" s="16"/>
@@ -5384,41 +5397,39 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>97</v>
+        <v>192</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>97</v>
+        <v>195</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J62" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J62" s="16"/>
       <c r="K62" s="16"/>
-      <c r="L62" s="16"/>
+      <c r="L62" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="16" t="s">
-        <v>220</v>
-      </c>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
       <c r="Q62" s="16"/>
       <c r="R62" s="16"/>
       <c r="S62" s="16"/>
@@ -5450,37 +5461,27 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="D63" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E63" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F63" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="G63" s="18" t="s">
-        <v>194</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
       <c r="H63" s="16"/>
-      <c r="I63" s="16" t="s">
-        <v>195</v>
-      </c>
+      <c r="I63" s="16"/>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
       <c r="O63" s="16"/>
-      <c r="P63" s="16"/>
+      <c r="P63" s="16" t="s">
+        <v>218</v>
+      </c>
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
       <c r="S63" s="16"/>
@@ -5512,39 +5513,27 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D64" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="E64" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="F64" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>200</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
       <c r="H64" s="16"/>
-      <c r="I64" s="16" t="s">
-        <v>196</v>
-      </c>
+      <c r="I64" s="16"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
-      <c r="L64" s="16" t="s">
-        <v>201</v>
-      </c>
+      <c r="L64" s="16"/>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
-      <c r="P64" s="16"/>
+      <c r="P64" s="16" t="s">
+        <v>220</v>
+      </c>
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="16"/>
@@ -5576,27 +5565,39 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
+        <v>198</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
+      <c r="I65" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
+      <c r="L65" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
       <c r="O65" s="16"/>
-      <c r="P65" s="16" t="s">
-        <v>222</v>
-      </c>
+      <c r="P65" s="16"/>
       <c r="Q65" s="16"/>
       <c r="R65" s="16"/>
       <c r="S65" s="16"/>
@@ -5631,7 +5632,7 @@
         <v>59</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
@@ -5647,7 +5648,7 @@
       <c r="N66" s="16"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
@@ -5680,39 +5681,27 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F67" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G67" s="18" t="s">
-        <v>28</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
       <c r="H67" s="16"/>
-      <c r="I67" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I67" s="16"/>
       <c r="J67" s="16"/>
       <c r="K67" s="16"/>
-      <c r="L67" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L67" s="16"/>
       <c r="M67" s="16"/>
       <c r="N67" s="16"/>
       <c r="O67" s="16"/>
-      <c r="P67" s="16"/>
+      <c r="P67" s="16" t="s">
+        <v>202</v>
+      </c>
       <c r="Q67" s="16"/>
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
@@ -5796,11 +5785,9 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>205</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B69" s="17"/>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
@@ -5814,9 +5801,7 @@
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
-      <c r="P69" s="16" t="s">
-        <v>206</v>
-      </c>
+      <c r="P69" s="16"/>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
@@ -5848,11 +5833,9 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>207</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B70" s="17"/>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
@@ -5866,9 +5849,7 @@
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
       <c r="O70" s="16"/>
-      <c r="P70" s="16" t="s">
-        <v>208</v>
-      </c>
+      <c r="P70" s="16"/>
       <c r="Q70" s="16"/>
       <c r="R70" s="16"/>
       <c r="S70" s="16"/>
@@ -5897,102 +5878,6 @@
       <c r="AP70" s="16"/>
       <c r="AQ70" s="16"/>
       <c r="AR70" s="16"/>
-    </row>
-    <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B71" s="17"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
-      <c r="M71" s="16"/>
-      <c r="N71" s="16"/>
-      <c r="O71" s="16"/>
-      <c r="P71" s="16"/>
-      <c r="Q71" s="16"/>
-      <c r="R71" s="16"/>
-      <c r="S71" s="16"/>
-      <c r="T71" s="16"/>
-      <c r="U71" s="16"/>
-      <c r="V71" s="16"/>
-      <c r="W71" s="16"/>
-      <c r="X71" s="16"/>
-      <c r="Y71" s="16"/>
-      <c r="Z71" s="16"/>
-      <c r="AA71" s="16"/>
-      <c r="AB71" s="16"/>
-      <c r="AC71" s="16"/>
-      <c r="AD71" s="16"/>
-      <c r="AE71" s="16"/>
-      <c r="AF71" s="16"/>
-      <c r="AG71" s="16"/>
-      <c r="AH71" s="16"/>
-      <c r="AI71" s="16"/>
-      <c r="AJ71" s="16"/>
-      <c r="AK71" s="16"/>
-      <c r="AL71" s="16"/>
-      <c r="AM71" s="16"/>
-      <c r="AN71" s="16"/>
-      <c r="AO71" s="16"/>
-      <c r="AP71" s="16"/>
-      <c r="AQ71" s="16"/>
-      <c r="AR71" s="16"/>
-    </row>
-    <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B72" s="17"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="16"/>
-      <c r="J72" s="16"/>
-      <c r="K72" s="16"/>
-      <c r="L72" s="16"/>
-      <c r="M72" s="16"/>
-      <c r="N72" s="16"/>
-      <c r="O72" s="16"/>
-      <c r="P72" s="16"/>
-      <c r="Q72" s="16"/>
-      <c r="R72" s="16"/>
-      <c r="S72" s="16"/>
-      <c r="T72" s="16"/>
-      <c r="U72" s="16"/>
-      <c r="V72" s="16"/>
-      <c r="W72" s="16"/>
-      <c r="X72" s="16"/>
-      <c r="Y72" s="16"/>
-      <c r="Z72" s="16"/>
-      <c r="AA72" s="16"/>
-      <c r="AB72" s="16"/>
-      <c r="AC72" s="16"/>
-      <c r="AD72" s="16"/>
-      <c r="AE72" s="16"/>
-      <c r="AF72" s="16"/>
-      <c r="AG72" s="16"/>
-      <c r="AH72" s="16"/>
-      <c r="AI72" s="16"/>
-      <c r="AJ72" s="16"/>
-      <c r="AK72" s="16"/>
-      <c r="AL72" s="16"/>
-      <c r="AM72" s="16"/>
-      <c r="AN72" s="16"/>
-      <c r="AO72" s="16"/>
-      <c r="AP72" s="16"/>
-      <c r="AQ72" s="16"/>
-      <c r="AR72" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -6027,13 +5912,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -6073,30 +5958,30 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="26" t="s">
+      <c r="G2" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="H2" s="31"/>
+      <c r="I2" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -6117,30 +6002,30 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="G3" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="19" t="s">
         <v>235</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="19" t="s">
-        <v>239</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6161,30 +6046,30 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>240</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="F4" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="G4" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="H4" s="31"/>
+      <c r="I4" s="19" t="s">
         <v>243</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="19" t="s">
-        <v>247</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -6205,30 +6090,30 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="G5" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="H5" s="31"/>
+      <c r="I5" s="19" t="s">
         <v>250</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="19" t="s">
-        <v>254</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -6249,30 +6134,30 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="G6" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="H6" s="31"/>
+      <c r="I6" s="19" t="s">
         <v>257</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>260</v>
-      </c>
-      <c r="H6" s="30"/>
-      <c r="I6" s="19" t="s">
-        <v>261</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -6293,30 +6178,30 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="G7" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="H7" s="31"/>
+      <c r="I7" s="19" t="s">
         <v>264</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>266</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="19" t="s">
-        <v>268</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -6337,30 +6222,30 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="G8" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="19" t="s">
         <v>271</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>273</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="19" t="s">
-        <v>275</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -6382,19 +6267,19 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>278</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+        <v>272</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -6416,29 +6301,29 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>279</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="F10" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="G10" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="H10" s="31"/>
+      <c r="I10" s="19" t="s">
         <v>282</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="H10" s="30"/>
-      <c r="I10" s="19" t="s">
-        <v>286</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -6460,29 +6345,29 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B11" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="G11" s="30" t="s">
         <v>288</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="H11" s="31"/>
+      <c r="I11" s="19" t="s">
         <v>289</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>291</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="19" t="s">
-        <v>293</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -6504,29 +6389,29 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="F12" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="G12" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>296</v>
-      </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="19" t="s">
-        <v>299</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6548,29 +6433,29 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B13" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="29" t="s">
         <v>300</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="G13" s="30" t="s">
         <v>301</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="H13" s="31"/>
+      <c r="I13" s="19" t="s">
         <v>302</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="19" t="s">
-        <v>306</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -6592,29 +6477,29 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="F14" s="29" t="s">
         <v>307</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="G14" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="D14" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>311</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="19" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -6636,29 +6521,29 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B15" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="F15" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="G15" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="H15" s="31"/>
+      <c r="I15" s="19" t="s">
         <v>314</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="19" t="s">
-        <v>318</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -6679,30 +6564,30 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="D16" s="27" t="s">
+      <c r="A16" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="H16" s="31"/>
+      <c r="I16" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -6723,30 +6608,30 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="E17" s="33" t="s">
         <v>319</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="F17" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="G17" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="H17" s="31"/>
+      <c r="I17" s="19" t="s">
         <v>322</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>324</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>325</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="19" t="s">
-        <v>326</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -6770,27 +6655,27 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="F18" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="G18" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="H18" s="31"/>
+      <c r="I18" s="19" t="s">
         <v>329</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>330</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="19" t="s">
-        <v>333</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6814,27 +6699,27 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="F19" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="G19" s="30" t="s">
         <v>335</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="H19" s="31"/>
+      <c r="I19" s="19" t="s">
         <v>336</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>338</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="19" t="s">
-        <v>340</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6858,27 +6743,27 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>338</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="G20" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="19" t="s">
         <v>342</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>343</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>344</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="19" t="s">
-        <v>346</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6902,27 +6787,27 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>327</v>
-      </c>
-      <c r="C21" s="34" t="s">
+      <c r="B21" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>344</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>345</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="G21" s="30" t="s">
         <v>347</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="H21" s="31"/>
+      <c r="I21" s="19" t="s">
         <v>348</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>349</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>350</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>351</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="19" t="s">
-        <v>352</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6946,27 +6831,27 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="C22" s="34" t="s">
+      <c r="B22" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>349</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="G22" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="H22" s="31"/>
+      <c r="I22" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>355</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>356</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>357</v>
-      </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="19" t="s">
-        <v>358</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -6990,27 +6875,27 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="G23" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="H23" s="31"/>
+      <c r="I23" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>362</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>363</v>
-      </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="19" t="s">
-        <v>364</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -7031,28 +6916,28 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="36" t="s">
-        <v>365</v>
-      </c>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="37" t="s">
+        <v>361</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
@@ -7108,19 +6993,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7145,20 +7030,20 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="C2" s="37" t="str">
+        <v>368</v>
+      </c>
+      <c r="C2" s="38" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-06-13 17-11</v>
+        <v xml:space="preserve">2022-08-15 11-54</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>

</xml_diff>

<commit_message>
Update default contact forms that had merge conflicts
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -161,7 +161,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>horizontal-compact</t>
+    <t>columns-pack</t>
   </si>
   <si>
     <t>db:person</t>
@@ -425,7 +425,7 @@
     <t>DELETE_THIS_LINE</t>
   </si>
   <si>
-    <t>horizontal</t>
+    <t>columns</t>
   </si>
   <si>
     <t>dob_approx</t>
@@ -1247,7 +1247,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1270,15 +1270,12 @@
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2424,7 +2421,7 @@
         <v>47</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="18" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="16"/>
@@ -2612,7 +2609,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="18" t="s">
+      <c r="P14" s="19" t="s">
         <v>61</v>
       </c>
       <c r="Q14" s="16"/>
@@ -2654,7 +2651,7 @@
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -2720,7 +2717,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="18"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2731,8 +2728,8 @@
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18" t="s">
+      <c r="O16" s="19"/>
+      <c r="P16" s="19" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="16"/>
@@ -2866,7 +2863,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="18"/>
+      <c r="P18" s="19"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
@@ -2875,7 +2872,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
-      <c r="Y18" s="18" t="s">
+      <c r="Y18" s="19" t="s">
         <v>79</v>
       </c>
       <c r="Z18" s="16"/>
@@ -2918,7 +2915,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="18" t="s">
+      <c r="P19" s="19" t="s">
         <v>81</v>
       </c>
       <c r="Q19" s="16"/>
@@ -2993,7 +2990,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="18" t="s">
+      <c r="Y20" s="19" t="s">
         <v>79</v>
       </c>
       <c r="Z20" s="16"/>
@@ -3036,7 +3033,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="18" t="s">
+      <c r="P21" s="19" t="s">
         <v>85</v>
       </c>
       <c r="Q21" s="16"/>
@@ -3244,7 +3241,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3308,7 +3305,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="19"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3360,7 +3357,7 @@
       <c r="C27" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="19" t="s">
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -3446,7 +3443,7 @@
       </c>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="20" t="s">
+      <c r="R28" s="21" t="s">
         <v>107</v>
       </c>
       <c r="S28" s="16"/>
@@ -3483,8 +3480,8 @@
       <c r="B29" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -3537,8 +3534,8 @@
       <c r="B30" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3592,20 +3589,20 @@
       <c r="C31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="19" t="s">
+      <c r="G31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19" t="s">
+      <c r="H31" s="20"/>
+      <c r="I31" s="20" t="s">
         <v>28</v>
       </c>
       <c r="J31" s="16"/>
@@ -3654,7 +3651,7 @@
       <c r="C32" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -3770,7 +3767,7 @@
       <c r="C34" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="18"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -3830,7 +3827,7 @@
       <c r="C35" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="18"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -3888,7 +3885,7 @@
       <c r="C36" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="18"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -3896,7 +3893,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="16" t="s">
+      <c r="L36" s="18" t="s">
         <v>136</v>
       </c>
       <c r="M36" s="16"/>
@@ -3942,7 +3939,7 @@
       <c r="C37" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="18"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -3954,7 +3951,7 @@
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
-      <c r="P37" s="21" t="s">
+      <c r="P37" s="16" t="s">
         <v>139</v>
       </c>
       <c r="Q37" s="16"/>
@@ -3994,7 +3991,7 @@
         <v>140</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="18"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -4048,7 +4045,7 @@
       <c r="C39" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="18"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -4099,10 +4096,10 @@
       <c r="B40" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="18"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
@@ -4153,7 +4150,7 @@
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="16"/>
-      <c r="D41" s="18"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -4227,7 +4224,7 @@
       </c>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="24" t="b">
+      <c r="N42" s="23" t="b">
         <f t="shared" ref="N42:N43" si="0">TRUE()</f>
         <v>1</v>
       </c>
@@ -4296,7 +4293,7 @@
       </c>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="24" t="b">
+      <c r="N43" s="23" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4365,7 +4362,7 @@
       <c r="K44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L44" s="16" t="s">
+      <c r="L44" s="18" t="s">
         <v>136</v>
       </c>
       <c r="M44" s="16"/>
@@ -5072,7 +5069,7 @@
       <c r="AR56" s="16"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B57" s="17" t="s">
@@ -5136,7 +5133,7 @@
       <c r="AR57" s="16"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="17" t="s">
@@ -5229,7 +5226,7 @@
       <c r="K59" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="L59" s="16" t="s">
+      <c r="L59" s="18" t="s">
         <v>48</v>
       </c>
       <c r="M59" s="16"/>
@@ -5277,7 +5274,7 @@
       <c r="C60" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="D60" s="18" t="s">
+      <c r="D60" s="19" t="s">
         <v>97</v>
       </c>
       <c r="E60" s="16" t="s">
@@ -5352,7 +5349,7 @@
       <c r="F61" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="G61" s="18" t="s">
+      <c r="G61" s="19" t="s">
         <v>190</v>
       </c>
       <c r="H61" s="16"/>
@@ -5414,7 +5411,7 @@
       <c r="F62" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="G62" s="18" t="s">
+      <c r="G62" s="19" t="s">
         <v>196</v>
       </c>
       <c r="H62" s="16"/>
@@ -5582,7 +5579,7 @@
       <c r="F65" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G65" s="18" t="s">
+      <c r="G65" s="19" t="s">
         <v>28</v>
       </c>
       <c r="H65" s="16"/>
@@ -5912,13 +5909,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5958,29 +5955,29 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>224</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="19" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="20" t="s">
         <v>228</v>
       </c>
       <c r="J2" s="8"/>
@@ -6002,29 +5999,29 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>231</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="H3" s="31"/>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="20" t="s">
         <v>235</v>
       </c>
       <c r="J3" s="8"/>
@@ -6046,29 +6043,29 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="19" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="20" t="s">
         <v>243</v>
       </c>
       <c r="J4" s="8"/>
@@ -6090,29 +6087,29 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="19" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="20" t="s">
         <v>250</v>
       </c>
       <c r="J5" s="8"/>
@@ -6134,29 +6131,29 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="H6" s="31"/>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="20" t="s">
         <v>257</v>
       </c>
       <c r="J6" s="8"/>
@@ -6178,29 +6175,29 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="20" t="s">
         <v>264</v>
       </c>
       <c r="J7" s="8"/>
@@ -6222,29 +6219,29 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="28" t="s">
         <v>269</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="30"/>
+      <c r="I8" s="20" t="s">
         <v>271</v>
       </c>
       <c r="J8" s="8"/>
@@ -6269,18 +6266,18 @@
       <c r="A9" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="19"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -6303,26 +6300,26 @@
       <c r="A10" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="19" t="s">
+      <c r="H10" s="30"/>
+      <c r="I10" s="20" t="s">
         <v>282</v>
       </c>
       <c r="J10" s="8"/>
@@ -6347,26 +6344,26 @@
       <c r="A11" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>283</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="32" t="s">
         <v>286</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="19" t="s">
+      <c r="H11" s="30"/>
+      <c r="I11" s="20" t="s">
         <v>289</v>
       </c>
       <c r="J11" s="8"/>
@@ -6391,26 +6388,26 @@
       <c r="A12" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="28" t="s">
         <v>294</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="19" t="s">
+      <c r="H12" s="30"/>
+      <c r="I12" s="20" t="s">
         <v>295</v>
       </c>
       <c r="J12" s="8"/>
@@ -6435,26 +6432,26 @@
       <c r="A13" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="28" t="s">
         <v>300</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="19" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="20" t="s">
         <v>302</v>
       </c>
       <c r="J13" s="8"/>
@@ -6485,20 +6482,20 @@
       <c r="C14" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="27" t="s">
         <v>305</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="19" t="s">
+      <c r="H14" s="30"/>
+      <c r="I14" s="20" t="s">
         <v>304</v>
       </c>
       <c r="J14" s="8"/>
@@ -6523,26 +6520,26 @@
       <c r="A15" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>309</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="34" t="s">
         <v>310</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="19" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="20" t="s">
         <v>314</v>
       </c>
       <c r="J15" s="8"/>
@@ -6564,29 +6561,29 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>224</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="19" t="s">
+      <c r="H16" s="30"/>
+      <c r="I16" s="20" t="s">
         <v>228</v>
       </c>
       <c r="J16" s="8"/>
@@ -6608,29 +6605,29 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="30"/>
+      <c r="I17" s="20" t="s">
         <v>322</v>
       </c>
       <c r="J17" s="8"/>
@@ -6655,26 +6652,26 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="28" t="s">
         <v>327</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="19" t="s">
+      <c r="H18" s="30"/>
+      <c r="I18" s="20" t="s">
         <v>329</v>
       </c>
       <c r="J18" s="8"/>
@@ -6699,26 +6696,26 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="27" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="32" t="s">
         <v>333</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="20" t="s">
         <v>336</v>
       </c>
       <c r="J19" s="8"/>
@@ -6743,26 +6740,26 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
         <v>340</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="29" t="s">
         <v>339</v>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="19" t="s">
+      <c r="H20" s="30"/>
+      <c r="I20" s="20" t="s">
         <v>342</v>
       </c>
       <c r="J20" s="8"/>
@@ -6787,26 +6784,26 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="34" t="s">
         <v>343</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="30"/>
+      <c r="I21" s="20" t="s">
         <v>348</v>
       </c>
       <c r="J21" s="8"/>
@@ -6831,26 +6828,26 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="27" t="s">
         <v>350</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="H22" s="31"/>
-      <c r="I22" s="19" t="s">
+      <c r="H22" s="30"/>
+      <c r="I22" s="20" t="s">
         <v>354</v>
       </c>
       <c r="J22" s="8"/>
@@ -6875,26 +6872,26 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="34" t="s">
         <v>355</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G23" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="H23" s="31"/>
-      <c r="I23" s="19" t="s">
+      <c r="H23" s="30"/>
+      <c r="I23" s="20" t="s">
         <v>360</v>
       </c>
       <c r="J23" s="8"/>
@@ -6916,29 +6913,29 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="36" t="s">
         <v>361</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="19" t="s">
+      <c r="H24" s="30"/>
+      <c r="I24" s="20" t="s">
         <v>100</v>
       </c>
       <c r="J24" s="8"/>
@@ -7035,9 +7032,9 @@
       <c r="B2" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="C2" s="38" t="str">
+      <c r="C2" s="37" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-08-15 11-54</v>
+        <v xml:space="preserve">2022-08-24 11-44</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>369</v>

</xml_diff>

<commit_message>
Update default contact forms
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -368,7 +368,7 @@
     <t>not(selected(../dob_method,'approx'))</t>
   </si>
   <si>
-    <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today()))</t>
+    <t xml:space="preserve">. &lt;= now()</t>
   </si>
   <si>
     <t xml:space="preserve">Date must be before today</t>
@@ -1270,12 +1270,12 @@
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2421,7 +2421,7 @@
         <v>47</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="16" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="16"/>
@@ -2609,7 +2609,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Q14" s="16"/>
@@ -2651,7 +2651,7 @@
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -2717,7 +2717,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2728,8 +2728,8 @@
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19" t="s">
+      <c r="O16" s="18"/>
+      <c r="P16" s="18" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="16"/>
@@ -2863,7 +2863,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
@@ -2872,7 +2872,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
-      <c r="Y18" s="19" t="s">
+      <c r="Y18" s="18" t="s">
         <v>79</v>
       </c>
       <c r="Z18" s="16"/>
@@ -2915,7 +2915,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="18" t="s">
         <v>81</v>
       </c>
       <c r="Q19" s="16"/>
@@ -2990,7 +2990,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="19" t="s">
+      <c r="Y20" s="18" t="s">
         <v>79</v>
       </c>
       <c r="Z20" s="16"/>
@@ -3033,7 +3033,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="18" t="s">
         <v>85</v>
       </c>
       <c r="Q21" s="16"/>
@@ -3241,7 +3241,7 @@
       <c r="G25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="20"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="16" t="s">
         <v>28</v>
       </c>
@@ -3305,7 +3305,7 @@
       <c r="G26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="20"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="16" t="s">
         <v>28</v>
       </c>
@@ -3357,7 +3357,7 @@
       <c r="C27" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="21" t="s">
+      <c r="R28" s="20" t="s">
         <v>107</v>
       </c>
       <c r="S28" s="16"/>
@@ -3480,8 +3480,8 @@
       <c r="B29" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -3534,8 +3534,8 @@
       <c r="B30" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3589,20 +3589,20 @@
       <c r="C31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20" t="s">
+      <c r="H31" s="19"/>
+      <c r="I31" s="19" t="s">
         <v>28</v>
       </c>
       <c r="J31" s="16"/>
@@ -3651,7 +3651,7 @@
       <c r="C32" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
-      <c r="N32" s="16" t="s">
+      <c r="N32" s="21" t="s">
         <v>117</v>
       </c>
       <c r="O32" s="16" t="s">
@@ -3767,7 +3767,7 @@
       <c r="C34" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -3827,7 +3827,7 @@
       <c r="C35" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -3885,7 +3885,7 @@
       <c r="C36" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -3893,7 +3893,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="18" t="s">
+      <c r="L36" s="16" t="s">
         <v>136</v>
       </c>
       <c r="M36" s="16"/>
@@ -3939,7 +3939,7 @@
       <c r="C37" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D37" s="19"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -3991,7 +3991,7 @@
         <v>140</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -4045,7 +4045,7 @@
       <c r="C39" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -4099,7 +4099,7 @@
       <c r="C40" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="19"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="16"/>
-      <c r="D41" s="19"/>
+      <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -4362,7 +4362,7 @@
       <c r="K44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L44" s="18" t="s">
+      <c r="L44" s="16" t="s">
         <v>136</v>
       </c>
       <c r="M44" s="16"/>
@@ -5226,7 +5226,7 @@
       <c r="K59" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="L59" s="18" t="s">
+      <c r="L59" s="16" t="s">
         <v>48</v>
       </c>
       <c r="M59" s="16"/>
@@ -5274,7 +5274,7 @@
       <c r="C60" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="18" t="s">
         <v>97</v>
       </c>
       <c r="E60" s="16" t="s">
@@ -5349,7 +5349,7 @@
       <c r="F61" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="18" t="s">
         <v>190</v>
       </c>
       <c r="H61" s="16"/>
@@ -5411,7 +5411,7 @@
       <c r="F62" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="G62" s="19" t="s">
+      <c r="G62" s="18" t="s">
         <v>196</v>
       </c>
       <c r="H62" s="16"/>
@@ -5579,7 +5579,7 @@
       <c r="F65" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G65" s="19" t="s">
+      <c r="G65" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H65" s="16"/>
@@ -5977,7 +5977,7 @@
         <v>227</v>
       </c>
       <c r="H2" s="30"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>228</v>
       </c>
       <c r="J2" s="8"/>
@@ -6021,7 +6021,7 @@
         <v>234</v>
       </c>
       <c r="H3" s="30"/>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>235</v>
       </c>
       <c r="J3" s="8"/>
@@ -6065,7 +6065,7 @@
         <v>242</v>
       </c>
       <c r="H4" s="30"/>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>243</v>
       </c>
       <c r="J4" s="8"/>
@@ -6109,7 +6109,7 @@
         <v>249</v>
       </c>
       <c r="H5" s="30"/>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>250</v>
       </c>
       <c r="J5" s="8"/>
@@ -6153,7 +6153,7 @@
         <v>256</v>
       </c>
       <c r="H6" s="30"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>257</v>
       </c>
       <c r="J6" s="8"/>
@@ -6197,7 +6197,7 @@
         <v>263</v>
       </c>
       <c r="H7" s="30"/>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>264</v>
       </c>
       <c r="J7" s="8"/>
@@ -6241,7 +6241,7 @@
         <v>270</v>
       </c>
       <c r="H8" s="30"/>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>271</v>
       </c>
       <c r="J8" s="8"/>
@@ -6277,7 +6277,7 @@
       <c r="F9" s="28"/>
       <c r="G9" s="29"/>
       <c r="H9" s="30"/>
-      <c r="I9" s="20"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -6319,7 +6319,7 @@
         <v>281</v>
       </c>
       <c r="H10" s="30"/>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>282</v>
       </c>
       <c r="J10" s="8"/>
@@ -6363,7 +6363,7 @@
         <v>288</v>
       </c>
       <c r="H11" s="30"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="19" t="s">
         <v>289</v>
       </c>
       <c r="J11" s="8"/>
@@ -6407,7 +6407,7 @@
         <v>292</v>
       </c>
       <c r="H12" s="30"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="19" t="s">
         <v>295</v>
       </c>
       <c r="J12" s="8"/>
@@ -6451,7 +6451,7 @@
         <v>301</v>
       </c>
       <c r="H13" s="30"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="19" t="s">
         <v>302</v>
       </c>
       <c r="J13" s="8"/>
@@ -6495,7 +6495,7 @@
         <v>308</v>
       </c>
       <c r="H14" s="30"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="19" t="s">
         <v>304</v>
       </c>
       <c r="J14" s="8"/>
@@ -6539,7 +6539,7 @@
         <v>311</v>
       </c>
       <c r="H15" s="30"/>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>314</v>
       </c>
       <c r="J15" s="8"/>
@@ -6583,7 +6583,7 @@
         <v>316</v>
       </c>
       <c r="H16" s="30"/>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="19" t="s">
         <v>228</v>
       </c>
       <c r="J16" s="8"/>
@@ -6627,7 +6627,7 @@
         <v>321</v>
       </c>
       <c r="H17" s="30"/>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="19" t="s">
         <v>322</v>
       </c>
       <c r="J17" s="8"/>
@@ -6671,7 +6671,7 @@
         <v>328</v>
       </c>
       <c r="H18" s="30"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>329</v>
       </c>
       <c r="J18" s="8"/>
@@ -6715,7 +6715,7 @@
         <v>335</v>
       </c>
       <c r="H19" s="30"/>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>336</v>
       </c>
       <c r="J19" s="8"/>
@@ -6759,7 +6759,7 @@
         <v>339</v>
       </c>
       <c r="H20" s="30"/>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>342</v>
       </c>
       <c r="J20" s="8"/>
@@ -6803,7 +6803,7 @@
         <v>347</v>
       </c>
       <c r="H21" s="30"/>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>348</v>
       </c>
       <c r="J21" s="8"/>
@@ -6847,7 +6847,7 @@
         <v>353</v>
       </c>
       <c r="H22" s="30"/>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>354</v>
       </c>
       <c r="J22" s="8"/>
@@ -6891,7 +6891,7 @@
         <v>359</v>
       </c>
       <c r="H23" s="30"/>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>360</v>
       </c>
       <c r="J23" s="8"/>
@@ -6935,7 +6935,7 @@
         <v>97</v>
       </c>
       <c r="H24" s="30"/>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
       <c r="J24" s="8"/>
@@ -7034,7 +7034,7 @@
       </c>
       <c r="C2" s="37" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-08-24 11-44</v>
+        <v xml:space="preserve">2022-09-26 12-17</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>369</v>

</xml_diff>

<commit_message>
Revert "Update default/standard config forms to pass validation (#7739)"
This reverts commit 7decc21661ac1bb549292b250af290ed2014370b.
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
   <si>
     <t>type</t>
   </si>
@@ -161,7 +161,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>columns-pack</t>
+    <t>horizontal-compact</t>
   </si>
   <si>
     <t>db:person</t>
@@ -425,7 +425,19 @@
     <t>DELETE_THIS_LINE</t>
   </si>
   <si>
-    <t>columns</t>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>ephemeral_months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(format-date-time(today(),"%m") - ../age_months &lt; 0, format-date-time(today(),"%m") - ../age_months + 12, format-date-time(today(),"%m") - ../age_months)</t>
+  </si>
+  <si>
+    <t>ephemeral_years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(format-date-time(today(),"%m") - ../age_months &lt; 0, format-date-time(today(),"%Y") - ../age_years - 1, format-date-time(today(),"%Y") -../age_years)</t>
   </si>
   <si>
     <t>dob_approx</t>
@@ -434,7 +446,7 @@
     <t>DOB</t>
   </si>
   <si>
-    <t xml:space="preserve">add-date(today(), 0-${age_years}, 0-${age_months})</t>
+    <t xml:space="preserve">concat(string(${ephemeral_years}),'-',if(${ephemeral_months}&lt;10, concat('0',string(${ephemeral_months})), ${ephemeral_months}),'-',string(format-date-time(today(), "%d")))</t>
   </si>
   <si>
     <t>dob_raw</t>
@@ -454,7 +466,9 @@
     <t>dob_debug</t>
   </si>
   <si>
-    <t xml:space="preserve">DOB Approx: ${dob_approx}
+    <t xml:space="preserve">Months: ${ephemeral_months}
+Year: ${ephemeral_years}
+DOB Approx: ${dob_approx}
 DOB Calendar: ${dob_calendar}
 DOB ISO: ${dob_iso}</t>
   </si>
@@ -1137,11 +1151,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <name val="Calibri"/>
-      <color theme="1"/>
+      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
     <font>
@@ -1151,6 +1165,7 @@
     <font>
       <name val="Calibri"/>
       <b/>
+      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
     <font>
@@ -1159,6 +1174,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
   </fonts>
@@ -1247,7 +1263,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1270,10 +1286,10 @@
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1285,6 +1301,7 @@
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1742,12 +1759,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" workbookViewId="0" zoomScale="100">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection activeCell="P39" activeCellId="0" sqref="P39"/>
     </sheetView>
   </sheetViews>
@@ -2421,7 +2438,7 @@
         <v>47</v>
       </c>
       <c r="K11" s="16"/>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="16" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="16"/>
@@ -2609,7 +2626,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Q14" s="16"/>
@@ -2651,7 +2668,7 @@
       <c r="C15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="16" t="s">
@@ -2668,7 +2685,7 @@
         <v>28</v>
       </c>
       <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="19" t="s">
         <v>64</v>
       </c>
       <c r="L15" s="16" t="s">
@@ -2717,7 +2734,7 @@
         <v>66</v>
       </c>
       <c r="C16" s="16"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -2728,8 +2745,8 @@
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19" t="s">
+      <c r="O16" s="18"/>
+      <c r="P16" s="18" t="s">
         <v>67</v>
       </c>
       <c r="Q16" s="16"/>
@@ -2790,7 +2807,7 @@
       <c r="J17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="K17" s="19" t="s">
         <v>64</v>
       </c>
       <c r="L17" s="16"/>
@@ -2863,7 +2880,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
-      <c r="P18" s="19"/>
+      <c r="P18" s="18"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="S18" s="16"/>
@@ -2872,7 +2889,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
       <c r="X18" s="16"/>
-      <c r="Y18" s="19" t="s">
+      <c r="Y18" s="18" t="s">
         <v>79</v>
       </c>
       <c r="Z18" s="16"/>
@@ -2915,7 +2932,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="18" t="s">
         <v>81</v>
       </c>
       <c r="Q19" s="16"/>
@@ -2990,7 +3007,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
-      <c r="Y20" s="19" t="s">
+      <c r="Y20" s="18" t="s">
         <v>79</v>
       </c>
       <c r="Z20" s="16"/>
@@ -3033,7 +3050,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="18" t="s">
         <v>85</v>
       </c>
       <c r="Q21" s="16"/>
@@ -3357,7 +3374,7 @@
       <c r="C27" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="18" t="s">
         <v>97</v>
       </c>
       <c r="E27" s="16" t="s">
@@ -3481,7 +3498,7 @@
         <v>108</v>
       </c>
       <c r="C29" s="20"/>
-      <c r="D29" s="19"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -3535,7 +3552,7 @@
         <v>110</v>
       </c>
       <c r="C30" s="20"/>
-      <c r="D30" s="19"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3651,7 +3668,7 @@
       <c r="C32" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -3767,7 +3784,7 @@
       <c r="C34" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
@@ -3827,7 +3844,7 @@
       <c r="C35" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
@@ -3885,7 +3902,7 @@
       <c r="C36" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="19"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
@@ -3893,7 +3910,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="18" t="s">
+      <c r="L36" s="16" t="s">
         <v>136</v>
       </c>
       <c r="M36" s="16"/>
@@ -3936,10 +3953,8 @@
       <c r="B37" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="19"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
@@ -3952,7 +3967,7 @@
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
       <c r="P37" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -3988,10 +4003,10 @@
         <v>59</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="18"/>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -4003,8 +4018,8 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="22" t="s">
-        <v>141</v>
+      <c r="P38" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
@@ -4040,12 +4055,12 @@
         <v>59</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="19"/>
+      <c r="D39" s="18"/>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
@@ -4091,30 +4106,27 @@
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>120</v>
+        <v>59</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" s="19"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
-      <c r="K40" s="16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="K40" s="16"/>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
-      <c r="P40" s="16"/>
+      <c r="P40" s="22" t="s">
+        <v>145</v>
+      </c>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
       <c r="S40" s="16"/>
@@ -4146,11 +4158,15 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
@@ -4162,7 +4178,9 @@
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
-      <c r="P41" s="16"/>
+      <c r="P41" s="16" t="s">
+        <v>147</v>
+      </c>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
       <c r="S41" s="16"/>
@@ -4194,43 +4212,29 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="17" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C42" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="C42" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="G42" s="16" t="s">
-        <v>152</v>
-      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
       <c r="H42" s="16"/>
-      <c r="I42" s="16" t="s">
-        <v>153</v>
-      </c>
+      <c r="I42" s="16"/>
       <c r="J42" s="16"/>
-      <c r="K42" s="16" t="s">
-        <v>92</v>
+      <c r="K42" s="16">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="23" t="b">
-        <f t="shared" ref="N42:N43" si="0">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>154</v>
-      </c>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
@@ -4263,43 +4267,22 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>160</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B43" s="17"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
       <c r="H43" s="16"/>
-      <c r="I43" s="16" t="s">
-        <v>161</v>
-      </c>
+      <c r="I43" s="16"/>
       <c r="J43" s="16"/>
-      <c r="K43" s="16" t="s">
-        <v>92</v>
-      </c>
+      <c r="K43" s="16"/>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="23" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O43" s="16" t="s">
-        <v>154</v>
-      </c>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
@@ -4332,42 +4315,43 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="17" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="J44" s="16"/>
       <c r="K44" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="L44" s="18" t="s">
-        <v>136</v>
-      </c>
+      <c r="L44" s="16"/>
       <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
+      <c r="N44" s="23">
+        <f t="shared" ref="N44:N45" si="0">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O44" s="16" t="s">
+        <v>158</v>
+      </c>
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
@@ -4400,29 +4384,29 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="17" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="16" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="J45" s="16"/>
       <c r="K45" s="16" t="s">
@@ -4430,8 +4414,13 @@
       </c>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
+      <c r="N45" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O45" s="16" t="s">
+        <v>158</v>
+      </c>
       <c r="P45" s="16"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
@@ -4464,37 +4453,39 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="17" t="s">
-        <v>30</v>
+        <v>166</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="J46" s="16" t="s">
         <v>47</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="L46" s="16"/>
+        <v>92</v>
+      </c>
+      <c r="L46" s="16" t="s">
+        <v>136</v>
+      </c>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
       <c r="O46" s="16"/>
@@ -4530,29 +4521,29 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="17" t="s">
-        <v>30</v>
+        <v>173</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E47" s="16" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="J47" s="16"/>
       <c r="K47" s="16" t="s">
@@ -4597,34 +4588,34 @@
         <v>30</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>25</v>
+        <v>181</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="E48" s="16" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="J48" s="16"/>
+        <v>187</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K48" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="L48" s="16" t="s">
-        <v>197</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="L48" s="16"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
@@ -4660,25 +4651,35 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
+        <v>190</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>194</v>
+      </c>
       <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
+      <c r="I49" s="16" t="s">
+        <v>195</v>
+      </c>
       <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="K49" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
@@ -4714,27 +4715,41 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B50" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F50" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
+      <c r="G50" s="16" t="s">
+        <v>200</v>
+      </c>
       <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
+      <c r="I50" s="16" t="s">
+        <v>196</v>
+      </c>
       <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
+      <c r="K50" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="L50" s="16" t="s">
+        <v>201</v>
+      </c>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="16" t="s">
-        <v>200</v>
-      </c>
+      <c r="P50" s="16"/>
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
       <c r="S50" s="16"/>
@@ -4766,12 +4781,14 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" s="16"/>
+        <v>202</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
       <c r="F51" s="16"/>
@@ -4780,13 +4797,13 @@
       <c r="I51" s="16"/>
       <c r="J51" s="16"/>
       <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
+      <c r="L51" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
-      <c r="P51" s="16" t="s">
-        <v>202</v>
-      </c>
+      <c r="P51" s="16"/>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
       <c r="S51" s="16"/>
@@ -4870,9 +4887,11 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>205</v>
+      </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -4886,7 +4905,9 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
+      <c r="P53" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
       <c r="S53" s="16"/>
@@ -4918,9 +4939,11 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>207</v>
+      </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -4934,7 +4957,9 @@
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
-      <c r="P54" s="16"/>
+      <c r="P54" s="16" t="s">
+        <v>208</v>
+      </c>
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
       <c r="S54" s="16"/>
@@ -4965,76 +4990,68 @@
       <c r="AR54" s="16"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="15"/>
+      <c r="A55" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
       <c r="I55" s="16"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="13"/>
-      <c r="V55" s="14"/>
-      <c r="W55" s="15"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="16"/>
+      <c r="V55" s="16"/>
+      <c r="W55" s="16"/>
       <c r="X55" s="16"/>
-      <c r="Y55" s="8"/>
-      <c r="Z55" s="8"/>
-      <c r="AA55" s="8"/>
-      <c r="AB55" s="8"/>
-      <c r="AC55" s="8"/>
-      <c r="AD55" s="8"/>
-      <c r="AE55" s="8"/>
-      <c r="AF55" s="8"/>
-      <c r="AG55" s="8"/>
-      <c r="AH55" s="8"/>
-      <c r="AI55" s="8"/>
-      <c r="AJ55" s="8"/>
-      <c r="AK55" s="8"/>
-      <c r="AL55" s="8"/>
+      <c r="Y55" s="16"/>
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="16"/>
+      <c r="AB55" s="16"/>
+      <c r="AC55" s="16"/>
+      <c r="AD55" s="16"/>
+      <c r="AE55" s="16"/>
+      <c r="AF55" s="16"/>
+      <c r="AG55" s="16"/>
+      <c r="AH55" s="16"/>
+      <c r="AI55" s="16"/>
+      <c r="AJ55" s="16"/>
+      <c r="AK55" s="16"/>
+      <c r="AL55" s="16"/>
+      <c r="AM55" s="16"/>
+      <c r="AN55" s="16"/>
+      <c r="AO55" s="16"/>
+      <c r="AP55" s="16"/>
+      <c r="AQ55" s="16"/>
+      <c r="AR55" s="16"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>28</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B56" s="17"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I56" s="16"/>
       <c r="J56" s="16"/>
       <c r="K56" s="16"/>
-      <c r="L56" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="L56" s="16"/>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
       <c r="O56" s="16"/>
@@ -5069,75 +5086,51 @@
       <c r="AR56" s="16"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="16"/>
-      <c r="O57" s="16"/>
-      <c r="P57" s="16"/>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="16"/>
-      <c r="S57" s="16"/>
-      <c r="T57" s="16"/>
-      <c r="U57" s="16"/>
-      <c r="V57" s="16"/>
-      <c r="W57" s="16"/>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="8"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="12"/>
+      <c r="U57" s="13"/>
+      <c r="V57" s="14"/>
+      <c r="W57" s="15"/>
       <c r="X57" s="16"/>
-      <c r="Y57" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z57" s="16"/>
-      <c r="AA57" s="16"/>
-      <c r="AB57" s="16"/>
-      <c r="AC57" s="16"/>
-      <c r="AD57" s="16"/>
-      <c r="AE57" s="16"/>
-      <c r="AF57" s="16"/>
-      <c r="AG57" s="16"/>
-      <c r="AH57" s="16"/>
-      <c r="AI57" s="16"/>
-      <c r="AJ57" s="16"/>
-      <c r="AK57" s="16"/>
-      <c r="AL57" s="16"/>
-      <c r="AM57" s="16"/>
-      <c r="AN57" s="16"/>
-      <c r="AO57" s="16"/>
-      <c r="AP57" s="16"/>
-      <c r="AQ57" s="16"/>
-      <c r="AR57" s="16"/>
+      <c r="Y57" s="8"/>
+      <c r="Z57" s="8"/>
+      <c r="AA57" s="8"/>
+      <c r="AB57" s="8"/>
+      <c r="AC57" s="8"/>
+      <c r="AD57" s="8"/>
+      <c r="AE57" s="8"/>
+      <c r="AF57" s="8"/>
+      <c r="AG57" s="8"/>
+      <c r="AH57" s="8"/>
+      <c r="AI57" s="8"/>
+      <c r="AJ57" s="8"/>
+      <c r="AK57" s="8"/>
+      <c r="AL57" s="8"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="24" t="s">
-        <v>58</v>
+      <c r="A58" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>28</v>
@@ -5160,7 +5153,9 @@
       </c>
       <c r="J58" s="16"/>
       <c r="K58" s="16"/>
-      <c r="L58" s="16"/>
+      <c r="L58" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
       <c r="O58" s="16"/>
@@ -5195,40 +5190,34 @@
       <c r="AR58" s="16"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="17" t="s">
-        <v>205</v>
+      <c r="A59" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>206</v>
+        <v>93</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>207</v>
+        <v>28</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>209</v>
+        <v>28</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>210</v>
+        <v>28</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>211</v>
+        <v>28</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K59" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="L59" s="18" t="s">
-        <v>48</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
@@ -5242,7 +5231,7 @@
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
       <c r="Y59" s="16" t="s">
-        <v>214</v>
+        <v>94</v>
       </c>
       <c r="Z59" s="16"/>
       <c r="AA59" s="16"/>
@@ -5265,42 +5254,38 @@
       <c r="AR59" s="16"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="17" t="s">
-        <v>59</v>
+      <c r="A60" s="24" t="s">
+        <v>58</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>97</v>
+        <v>28</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J60" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J60" s="16"/>
       <c r="K60" s="16"/>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="16" t="s">
-        <v>216</v>
-      </c>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="16"/>
@@ -5331,34 +5316,40 @@
       <c r="AR60" s="16"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="17" t="s">
-        <v>30</v>
+      <c r="A61" s="25" t="s">
+        <v>209</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>190</v>
+        <v>214</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="16"/>
+        <v>216</v>
+      </c>
+      <c r="J61" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K61" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="L61" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
       <c r="O61" s="16"/>
@@ -5371,7 +5362,9 @@
       <c r="V61" s="16"/>
       <c r="W61" s="16"/>
       <c r="X61" s="16"/>
-      <c r="Y61" s="16"/>
+      <c r="Y61" s="16" t="s">
+        <v>218</v>
+      </c>
       <c r="Z61" s="16"/>
       <c r="AA61" s="16"/>
       <c r="AB61" s="16"/>
@@ -5394,39 +5387,41 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="D62" s="16" t="s">
-        <v>193</v>
+        <v>219</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>194</v>
+        <v>98</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="G62" s="19" t="s">
-        <v>196</v>
+        <v>99</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="J62" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="J62" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K62" s="16"/>
-      <c r="L62" s="16" t="s">
-        <v>197</v>
-      </c>
+      <c r="L62" s="16"/>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
-      <c r="O62" s="16"/>
-      <c r="P62" s="16"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="16" t="s">
+        <v>220</v>
+      </c>
       <c r="Q62" s="16"/>
       <c r="R62" s="16"/>
       <c r="S62" s="16"/>
@@ -5458,27 +5453,37 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+        <v>189</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>194</v>
+      </c>
       <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
+      <c r="I63" s="16" t="s">
+        <v>195</v>
+      </c>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
       <c r="O63" s="16"/>
-      <c r="P63" s="16" t="s">
-        <v>218</v>
-      </c>
+      <c r="P63" s="16"/>
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
       <c r="S63" s="16"/>
@@ -5510,27 +5515,39 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>200</v>
+      </c>
       <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
+      <c r="I64" s="16" t="s">
+        <v>196</v>
+      </c>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
+      <c r="L64" s="16" t="s">
+        <v>201</v>
+      </c>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
-      <c r="P64" s="16" t="s">
-        <v>220</v>
-      </c>
+      <c r="P64" s="16"/>
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="16"/>
@@ -5562,39 +5579,27 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>28</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
       <c r="H65" s="16"/>
-      <c r="I65" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I65" s="16"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
-      <c r="L65" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L65" s="16"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
       <c r="O65" s="16"/>
-      <c r="P65" s="16"/>
+      <c r="P65" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="Q65" s="16"/>
       <c r="R65" s="16"/>
       <c r="S65" s="16"/>
@@ -5629,7 +5634,7 @@
         <v>59</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
@@ -5645,7 +5650,7 @@
       <c r="N66" s="16"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
@@ -5678,27 +5683,39 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
+        <v>202</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G67" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
+      <c r="I67" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J67" s="16"/>
       <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
+      <c r="L67" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M67" s="16"/>
       <c r="N67" s="16"/>
       <c r="O67" s="16"/>
-      <c r="P67" s="16" t="s">
-        <v>202</v>
-      </c>
+      <c r="P67" s="16"/>
       <c r="Q67" s="16"/>
       <c r="R67" s="16"/>
       <c r="S67" s="16"/>
@@ -5782,9 +5799,11 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>205</v>
+      </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
@@ -5798,7 +5817,9 @@
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
-      <c r="P69" s="16"/>
+      <c r="P69" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
@@ -5830,9 +5851,11 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>207</v>
+      </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
@@ -5846,7 +5869,9 @@
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
       <c r="O70" s="16"/>
-      <c r="P70" s="16"/>
+      <c r="P70" s="16" t="s">
+        <v>208</v>
+      </c>
       <c r="Q70" s="16"/>
       <c r="R70" s="16"/>
       <c r="S70" s="16"/>
@@ -5876,10 +5901,106 @@
       <c r="AQ70" s="16"/>
       <c r="AR70" s="16"/>
     </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="17"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
+      <c r="M71" s="16"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="16"/>
+      <c r="P71" s="16"/>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+      <c r="T71" s="16"/>
+      <c r="U71" s="16"/>
+      <c r="V71" s="16"/>
+      <c r="W71" s="16"/>
+      <c r="X71" s="16"/>
+      <c r="Y71" s="16"/>
+      <c r="Z71" s="16"/>
+      <c r="AA71" s="16"/>
+      <c r="AB71" s="16"/>
+      <c r="AC71" s="16"/>
+      <c r="AD71" s="16"/>
+      <c r="AE71" s="16"/>
+      <c r="AF71" s="16"/>
+      <c r="AG71" s="16"/>
+      <c r="AH71" s="16"/>
+      <c r="AI71" s="16"/>
+      <c r="AJ71" s="16"/>
+      <c r="AK71" s="16"/>
+      <c r="AL71" s="16"/>
+      <c r="AM71" s="16"/>
+      <c r="AN71" s="16"/>
+      <c r="AO71" s="16"/>
+      <c r="AP71" s="16"/>
+      <c r="AQ71" s="16"/>
+      <c r="AR71" s="16"/>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="17"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
+      <c r="K72" s="16"/>
+      <c r="L72" s="16"/>
+      <c r="M72" s="16"/>
+      <c r="N72" s="16"/>
+      <c r="O72" s="16"/>
+      <c r="P72" s="16"/>
+      <c r="Q72" s="16"/>
+      <c r="R72" s="16"/>
+      <c r="S72" s="16"/>
+      <c r="T72" s="16"/>
+      <c r="U72" s="16"/>
+      <c r="V72" s="16"/>
+      <c r="W72" s="16"/>
+      <c r="X72" s="16"/>
+      <c r="Y72" s="16"/>
+      <c r="Z72" s="16"/>
+      <c r="AA72" s="16"/>
+      <c r="AB72" s="16"/>
+      <c r="AC72" s="16"/>
+      <c r="AD72" s="16"/>
+      <c r="AE72" s="16"/>
+      <c r="AF72" s="16"/>
+      <c r="AG72" s="16"/>
+      <c r="AH72" s="16"/>
+      <c r="AI72" s="16"/>
+      <c r="AJ72" s="16"/>
+      <c r="AK72" s="16"/>
+      <c r="AL72" s="16"/>
+      <c r="AM72" s="16"/>
+      <c r="AN72" s="16"/>
+      <c r="AO72" s="16"/>
+      <c r="AP72" s="16"/>
+      <c r="AQ72" s="16"/>
+      <c r="AR72" s="16"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -5887,11 +6008,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5909,13 +6030,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5955,30 +6076,30 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>224</v>
+      <c r="A2" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>228</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>229</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="H2" s="31"/>
       <c r="I2" s="20" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -5999,30 +6120,30 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>231</v>
+      <c r="A3" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>235</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="H3" s="30"/>
+        <v>236</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="H3" s="31"/>
       <c r="I3" s="20" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6043,30 +6164,30 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="E4" s="32" t="s">
+      <c r="A4" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="C4" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="30"/>
+      <c r="D4" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" s="31"/>
       <c r="I4" s="20" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -6087,30 +6208,30 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="F5" s="28" t="s">
+      <c r="A5" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="C5" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="30"/>
+      <c r="D5" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="H5" s="31"/>
       <c r="I5" s="20" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -6131,30 +6252,30 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="F6" s="28" t="s">
+      <c r="B6" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="C6" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="D6" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="H6" s="31"/>
       <c r="I6" s="20" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -6175,30 +6296,30 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="F7" s="28" t="s">
+      <c r="B7" s="34" t="s">
         <v>262</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="C7" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="D7" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="H7" s="31"/>
       <c r="I7" s="20" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -6219,30 +6340,30 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="F8" s="28" t="s">
+      <c r="B8" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="C8" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="D8" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="H8" s="31"/>
       <c r="I8" s="20" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -6264,19 +6385,19 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+        <v>276</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="20"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -6298,29 +6419,29 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>277</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="E10" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="B10" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="C10" s="35" t="s">
         <v>281</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="D10" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="H10" s="31"/>
       <c r="I10" s="20" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -6342,29 +6463,29 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>284</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>286</v>
-      </c>
-      <c r="F11" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="C11" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="D11" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="20" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -6386,29 +6507,29 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>291</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="F12" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="G12" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H12" s="30"/>
+      <c r="C12" s="35" t="s">
+        <v>295</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="H12" s="31"/>
       <c r="I12" s="20" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6430,29 +6551,29 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>298</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="F13" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="C13" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="H13" s="30"/>
+      <c r="D13" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>305</v>
+      </c>
+      <c r="H13" s="31"/>
       <c r="I13" s="20" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -6474,29 +6595,29 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>306</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>307</v>
-      </c>
-      <c r="G14" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="D14" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="H14" s="31"/>
       <c r="I14" s="20" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -6518,29 +6639,29 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="F15" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="C15" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>315</v>
+      </c>
+      <c r="H15" s="31"/>
       <c r="I15" s="20" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -6561,30 +6682,30 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>224</v>
+      <c r="A16" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>228</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="H16" s="30"/>
+        <v>229</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="H16" s="31"/>
       <c r="I16" s="20" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -6605,30 +6726,30 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>318</v>
-      </c>
-      <c r="E17" s="32" t="s">
+      <c r="A17" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="28" t="s">
-        <v>320</v>
-      </c>
-      <c r="G17" s="29" t="s">
+      <c r="B17" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="D17" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>325</v>
+      </c>
+      <c r="H17" s="31"/>
       <c r="I17" s="20" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -6652,27 +6773,27 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>324</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>325</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="F18" s="28" t="s">
+      <c r="B18" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="C18" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="D18" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="H18" s="31"/>
       <c r="I18" s="20" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6696,27 +6817,27 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>331</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>332</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>333</v>
-      </c>
-      <c r="F19" s="28" t="s">
+      <c r="B19" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="C19" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="D19" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="H19" s="31"/>
       <c r="I19" s="20" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6740,27 +6861,27 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>338</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="F20" s="28" t="s">
+      <c r="B20" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="G20" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="H20" s="30"/>
+      <c r="C20" s="35" t="s">
+        <v>342</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="H20" s="31"/>
       <c r="I20" s="20" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6784,27 +6905,27 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>343</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>344</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>345</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>346</v>
-      </c>
-      <c r="G21" s="29" t="s">
+      <c r="B21" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="C21" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="H21" s="30"/>
+      <c r="D21" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="H21" s="31"/>
       <c r="I21" s="20" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6828,27 +6949,27 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>352</v>
-      </c>
-      <c r="G22" s="29" t="s">
+      <c r="B22" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="D22" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>356</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="H22" s="31"/>
       <c r="I22" s="20" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -6872,27 +6993,27 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>355</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>356</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>357</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="G23" s="35" t="s">
+      <c r="B23" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="D23" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>362</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>363</v>
+      </c>
+      <c r="H23" s="31"/>
       <c r="I23" s="20" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -6913,28 +7034,28 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="36" t="s">
-        <v>361</v>
-      </c>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="20" t="s">
         <v>100</v>
       </c>
@@ -6959,7 +7080,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -6967,11 +7088,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" workbookViewId="0" zoomScale="100">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6990,19 +7111,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7027,20 +7148,20 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="C2" s="37" t="str">
+        <v>372</v>
+      </c>
+      <c r="C2" s="38" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-08-24 11-44</v>
+        <v xml:space="preserve">2022-01-19 16-22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -13732,7 +13853,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up default form changes
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="373">
   <si>
     <t>type</t>
   </si>
@@ -613,6 +613,12 @@
   </si>
   <si>
     <t>multiline</t>
+  </si>
+  <si>
+    <t>create_user_for_contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected( ${role},'chw') or selected( ${role},'chw_supervisor')</t>
   </si>
   <si>
     <t>meta</t>
@@ -1138,7 +1144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -1159,6 +1165,11 @@
     </font>
     <font>
       <name val="Arial"/>
+      <sz val="11.000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color indexed="64"/>
       <sz val="11.000000"/>
     </font>
   </fonts>
@@ -1247,7 +1258,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1275,12 +1286,17 @@
     </xf>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="5" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="5" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3665,7 +3681,7 @@
       </c>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
-      <c r="N32" s="21" t="s">
+      <c r="N32" s="16" t="s">
         <v>117</v>
       </c>
       <c r="O32" s="16" t="s">
@@ -4003,7 +4019,7 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="22" t="s">
+      <c r="P38" s="21" t="s">
         <v>141</v>
       </c>
       <c r="Q38" s="16"/>
@@ -4096,7 +4112,7 @@
       <c r="B40" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>145</v>
       </c>
       <c r="D40" s="18"/>
@@ -4224,7 +4240,7 @@
       </c>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="23" t="b">
+      <c r="N42" s="22" t="b">
         <f t="shared" ref="N42:N43" si="0">TRUE()</f>
         <v>1</v>
       </c>
@@ -4293,7 +4309,7 @@
       </c>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="23" t="b">
+      <c r="N43" s="22" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4659,15 +4675,13 @@
       <c r="AR48" s="16"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="C49" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="C49" s="16"/>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
       <c r="F49" s="16"/>
@@ -4676,13 +4690,13 @@
       <c r="I49" s="16"/>
       <c r="J49" s="16"/>
       <c r="K49" s="16"/>
-      <c r="L49" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
-      <c r="P49" s="16"/>
+      <c r="P49" s="24" t="s">
+        <v>199</v>
+      </c>
       <c r="Q49" s="16"/>
       <c r="R49" s="16"/>
       <c r="S49" s="16"/>
@@ -4714,12 +4728,14 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" s="16"/>
+        <v>200</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
       <c r="F50" s="16"/>
@@ -4728,13 +4744,13 @@
       <c r="I50" s="16"/>
       <c r="J50" s="16"/>
       <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
+      <c r="L50" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="16" t="s">
-        <v>200</v>
-      </c>
+      <c r="P50" s="16"/>
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
       <c r="S50" s="16"/>
@@ -4870,9 +4886,11 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>205</v>
+      </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -4886,7 +4904,9 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
+      <c r="P53" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
       <c r="S53" s="16"/>
@@ -4965,115 +4985,99 @@
       <c r="AR54" s="16"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="15"/>
+      <c r="A55" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="17"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
       <c r="I55" s="16"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="13"/>
-      <c r="V55" s="14"/>
-      <c r="W55" s="15"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="16"/>
+      <c r="V55" s="16"/>
+      <c r="W55" s="16"/>
       <c r="X55" s="16"/>
-      <c r="Y55" s="8"/>
-      <c r="Z55" s="8"/>
-      <c r="AA55" s="8"/>
-      <c r="AB55" s="8"/>
-      <c r="AC55" s="8"/>
-      <c r="AD55" s="8"/>
-      <c r="AE55" s="8"/>
-      <c r="AF55" s="8"/>
-      <c r="AG55" s="8"/>
-      <c r="AH55" s="8"/>
-      <c r="AI55" s="8"/>
-      <c r="AJ55" s="8"/>
-      <c r="AK55" s="8"/>
-      <c r="AL55" s="8"/>
+      <c r="Y55" s="16"/>
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="16"/>
+      <c r="AB55" s="16"/>
+      <c r="AC55" s="16"/>
+      <c r="AD55" s="16"/>
+      <c r="AE55" s="16"/>
+      <c r="AF55" s="16"/>
+      <c r="AG55" s="16"/>
+      <c r="AH55" s="16"/>
+      <c r="AI55" s="16"/>
+      <c r="AJ55" s="16"/>
+      <c r="AK55" s="16"/>
+      <c r="AL55" s="16"/>
+      <c r="AM55" s="16"/>
+      <c r="AN55" s="16"/>
+      <c r="AO55" s="16"/>
+      <c r="AP55" s="16"/>
+      <c r="AQ55" s="16"/>
+      <c r="AR55" s="16"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="13"/>
+      <c r="V56" s="14"/>
+      <c r="W56" s="15"/>
+      <c r="X56" s="16"/>
+      <c r="Y56" s="8"/>
+      <c r="Z56" s="8"/>
+      <c r="AA56" s="8"/>
+      <c r="AB56" s="8"/>
+      <c r="AC56" s="8"/>
+      <c r="AD56" s="8"/>
+      <c r="AE56" s="8"/>
+      <c r="AF56" s="8"/>
+      <c r="AG56" s="8"/>
+      <c r="AH56" s="8"/>
+      <c r="AI56" s="8"/>
+      <c r="AJ56" s="8"/>
+      <c r="AK56" s="8"/>
+      <c r="AL56" s="8"/>
+    </row>
+    <row r="57" ht="14.25" customHeight="1">
+      <c r="A57" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B57" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="16"/>
-      <c r="R56" s="16"/>
-      <c r="S56" s="16"/>
-      <c r="T56" s="16"/>
-      <c r="U56" s="16"/>
-      <c r="V56" s="16"/>
-      <c r="W56" s="16"/>
-      <c r="X56" s="16"/>
-      <c r="Y56" s="16"/>
-      <c r="Z56" s="16"/>
-      <c r="AA56" s="16"/>
-      <c r="AB56" s="16"/>
-      <c r="AC56" s="16"/>
-      <c r="AD56" s="16"/>
-      <c r="AE56" s="16"/>
-      <c r="AF56" s="16"/>
-      <c r="AG56" s="16"/>
-      <c r="AH56" s="16"/>
-      <c r="AI56" s="16"/>
-      <c r="AJ56" s="16"/>
-      <c r="AK56" s="16"/>
-      <c r="AL56" s="16"/>
-      <c r="AM56" s="16"/>
-      <c r="AN56" s="16"/>
-      <c r="AO56" s="16"/>
-      <c r="AP56" s="16"/>
-      <c r="AQ56" s="16"/>
-      <c r="AR56" s="16"/>
-    </row>
-    <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="C57" s="16" t="s">
         <v>28</v>
@@ -5096,7 +5100,9 @@
       </c>
       <c r="J57" s="16"/>
       <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
+      <c r="L57" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
       <c r="O57" s="16"/>
@@ -5109,9 +5115,7 @@
       <c r="V57" s="16"/>
       <c r="W57" s="16"/>
       <c r="X57" s="16"/>
-      <c r="Y57" s="16" t="s">
-        <v>94</v>
-      </c>
+      <c r="Y57" s="16"/>
       <c r="Z57" s="16"/>
       <c r="AA57" s="16"/>
       <c r="AB57" s="16"/>
@@ -5133,11 +5137,11 @@
       <c r="AR57" s="16"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="C58" s="16" t="s">
         <v>28</v>
@@ -5173,7 +5177,9 @@
       <c r="V58" s="16"/>
       <c r="W58" s="16"/>
       <c r="X58" s="16"/>
-      <c r="Y58" s="16"/>
+      <c r="Y58" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="Z58" s="16"/>
       <c r="AA58" s="16"/>
       <c r="AB58" s="16"/>
@@ -5195,40 +5201,34 @@
       <c r="AR58" s="16"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
-      <c r="A59" s="17" t="s">
-        <v>205</v>
+      <c r="A59" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>206</v>
+        <v>0</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>207</v>
+        <v>28</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>209</v>
+        <v>28</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>210</v>
+        <v>28</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>211</v>
+        <v>28</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K59" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="L59" s="16" t="s">
-        <v>48</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
       <c r="O59" s="16"/>
@@ -5241,9 +5241,7 @@
       <c r="V59" s="16"/>
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
-      <c r="Y59" s="16" t="s">
-        <v>214</v>
-      </c>
+      <c r="Y59" s="16"/>
       <c r="Z59" s="16"/>
       <c r="AA59" s="16"/>
       <c r="AB59" s="16"/>
@@ -5266,41 +5264,43 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="17" t="s">
-        <v>59</v>
+        <v>207</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>97</v>
+        <v>209</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>210</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>98</v>
+        <v>211</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>97</v>
+        <v>213</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16" t="s">
-        <v>100</v>
+        <v>214</v>
       </c>
       <c r="J60" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="K60" s="16"/>
-      <c r="L60" s="16"/>
+      <c r="K60" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="L60" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="16" t="s">
-        <v>216</v>
-      </c>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="16"/>
@@ -5309,7 +5309,9 @@
       <c r="V60" s="16"/>
       <c r="W60" s="16"/>
       <c r="X60" s="16"/>
-      <c r="Y60" s="16"/>
+      <c r="Y60" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="Z60" s="16"/>
       <c r="AA60" s="16"/>
       <c r="AB60" s="16"/>
@@ -5332,37 +5334,41 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="17" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>185</v>
+        <v>1</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>187</v>
+        <v>217</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>188</v>
+        <v>98</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>190</v>
+        <v>99</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="J61" s="16"/>
+        <v>100</v>
+      </c>
+      <c r="J61" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K61" s="16"/>
       <c r="L61" s="16"/>
       <c r="M61" s="16"/>
       <c r="N61" s="16"/>
-      <c r="O61" s="16"/>
-      <c r="P61" s="16"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="16" t="s">
+        <v>218</v>
+      </c>
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
       <c r="S61" s="16"/>
@@ -5397,32 +5403,30 @@
         <v>30</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J62" s="16"/>
       <c r="K62" s="16"/>
-      <c r="L62" s="16" t="s">
-        <v>197</v>
-      </c>
+      <c r="L62" s="16"/>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
       <c r="O62" s="16"/>
@@ -5458,27 +5462,39 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>196</v>
+      </c>
       <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
+      <c r="I63" s="16" t="s">
+        <v>192</v>
+      </c>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
+      <c r="L63" s="16" t="s">
+        <v>197</v>
+      </c>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
       <c r="O63" s="16"/>
-      <c r="P63" s="16" t="s">
-        <v>218</v>
-      </c>
+      <c r="P63" s="16"/>
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
       <c r="S63" s="16"/>
@@ -5513,7 +5529,7 @@
         <v>59</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>219</v>
+        <v>86</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="16"/>
@@ -5562,39 +5578,27 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F65" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G65" s="18" t="s">
-        <v>28</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
       <c r="H65" s="16"/>
-      <c r="I65" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I65" s="16"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
-      <c r="L65" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L65" s="16"/>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
       <c r="O65" s="16"/>
-      <c r="P65" s="16"/>
+      <c r="P65" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="Q65" s="16"/>
       <c r="R65" s="16"/>
       <c r="S65" s="16"/>
@@ -5626,27 +5630,39 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
+        <v>200</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
+      <c r="I66" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J66" s="16"/>
       <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
+      <c r="L66" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M66" s="16"/>
       <c r="N66" s="16"/>
       <c r="O66" s="16"/>
-      <c r="P66" s="16" t="s">
-        <v>200</v>
-      </c>
+      <c r="P66" s="16"/>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
       <c r="S66" s="16"/>
@@ -5782,9 +5798,11 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>205</v>
+      </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
@@ -5798,7 +5816,9 @@
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
-      <c r="P69" s="16"/>
+      <c r="P69" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
@@ -5876,6 +5896,54 @@
       <c r="AQ70" s="16"/>
       <c r="AR70" s="16"/>
     </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" s="17"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
+      <c r="M71" s="16"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="16"/>
+      <c r="P71" s="16"/>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+      <c r="T71" s="16"/>
+      <c r="U71" s="16"/>
+      <c r="V71" s="16"/>
+      <c r="W71" s="16"/>
+      <c r="X71" s="16"/>
+      <c r="Y71" s="16"/>
+      <c r="Z71" s="16"/>
+      <c r="AA71" s="16"/>
+      <c r="AB71" s="16"/>
+      <c r="AC71" s="16"/>
+      <c r="AD71" s="16"/>
+      <c r="AE71" s="16"/>
+      <c r="AF71" s="16"/>
+      <c r="AG71" s="16"/>
+      <c r="AH71" s="16"/>
+      <c r="AI71" s="16"/>
+      <c r="AJ71" s="16"/>
+      <c r="AK71" s="16"/>
+      <c r="AL71" s="16"/>
+      <c r="AM71" s="16"/>
+      <c r="AN71" s="16"/>
+      <c r="AO71" s="16"/>
+      <c r="AP71" s="16"/>
+      <c r="AQ71" s="16"/>
+      <c r="AR71" s="16"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5909,13 +5977,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5955,30 +6023,30 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="A2" s="27" t="s">
         <v>224</v>
       </c>
+      <c r="B2" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>226</v>
+      </c>
       <c r="E2" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="H2" s="30"/>
+      <c r="F2" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="H2" s="31"/>
       <c r="I2" s="19" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -5999,30 +6067,30 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="A3" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>231</v>
       </c>
+      <c r="C3" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>233</v>
+      </c>
       <c r="E3" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="G3" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="H3" s="30"/>
+      <c r="F3" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" s="31"/>
       <c r="I3" s="19" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6043,30 +6111,30 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="B4" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="C4" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="D4" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="E4" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="30"/>
+      <c r="F4" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="H4" s="31"/>
       <c r="I4" s="19" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -6087,30 +6155,30 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5" s="31" t="s">
+      <c r="A5" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="C5" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="D5" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="E5" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="30"/>
+      <c r="F5" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="31"/>
       <c r="I5" s="19" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -6131,30 +6199,30 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" s="31" t="s">
+      <c r="B6" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="C6" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="D6" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="E6" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="F6" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="H6" s="31"/>
       <c r="I6" s="19" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -6175,30 +6243,30 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="B7" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="C7" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="D7" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="E7" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="F7" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="H7" s="31"/>
       <c r="I7" s="19" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -6219,30 +6287,30 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="B8" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="C8" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="D8" s="28" t="s">
         <v>269</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="E8" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="F8" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="H8" s="31"/>
       <c r="I8" s="19" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -6264,19 +6332,19 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+      <c r="B9" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -6298,29 +6366,29 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="B10" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="C10" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="D10" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="E10" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="F10" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="H10" s="31"/>
       <c r="I10" s="19" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -6342,29 +6410,29 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>284</v>
-      </c>
-      <c r="D11" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="C11" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="D11" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="E11" s="33" t="s">
         <v>288</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="F11" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="H11" s="31"/>
       <c r="I11" s="19" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -6386,29 +6454,29 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>291</v>
-      </c>
-      <c r="D12" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="C12" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="D12" s="28" t="s">
         <v>294</v>
       </c>
-      <c r="G12" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H12" s="30"/>
+      <c r="E12" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="H12" s="31"/>
       <c r="I12" s="19" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6430,29 +6498,29 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="C13" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="D13" s="28" t="s">
         <v>300</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="E13" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="H13" s="30"/>
+      <c r="F13" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="H13" s="31"/>
       <c r="I13" s="19" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -6474,29 +6542,29 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="E14" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="D14" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="E14" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="F14" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="H14" s="31"/>
       <c r="I14" s="19" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -6518,29 +6586,29 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="C15" s="35" t="s">
         <v>312</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="D15" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="E15" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="H15" s="31"/>
       <c r="I15" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -6561,30 +6629,30 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>224</v>
+      <c r="A16" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>226</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="H16" s="30"/>
+        <v>227</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="H16" s="31"/>
       <c r="I16" s="19" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -6605,30 +6673,30 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" s="26" t="s">
+      <c r="A17" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="D17" s="27" t="s">
-        <v>318</v>
-      </c>
-      <c r="E17" s="32" t="s">
+      <c r="B17" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="D17" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="E17" s="33" t="s">
         <v>321</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="F17" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="H17" s="31"/>
       <c r="I17" s="19" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -6652,27 +6720,27 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>324</v>
-      </c>
-      <c r="D18" s="27" t="s">
+      <c r="B18" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="C18" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="D18" s="28" t="s">
         <v>327</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="E18" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="F18" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="H18" s="31"/>
       <c r="I18" s="19" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6696,27 +6764,27 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>331</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="B19" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="C19" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="D19" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="E19" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="F19" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="H19" s="31"/>
       <c r="I19" s="19" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6740,27 +6808,27 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>338</v>
-      </c>
-      <c r="D20" s="27" t="s">
+      <c r="B20" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="C20" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="D20" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="G20" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="H20" s="30"/>
+      <c r="E20" s="33" t="s">
+        <v>342</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>341</v>
+      </c>
+      <c r="H20" s="31"/>
       <c r="I20" s="19" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6784,27 +6852,27 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>343</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>344</v>
-      </c>
-      <c r="E21" s="32" t="s">
+      <c r="B21" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C21" s="35" t="s">
         <v>345</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="D21" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="E21" s="33" t="s">
         <v>347</v>
       </c>
-      <c r="H21" s="30"/>
+      <c r="F21" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="H21" s="31"/>
       <c r="I21" s="19" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6828,27 +6896,27 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="E22" s="32" t="s">
+      <c r="B22" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="C22" s="35" t="s">
         <v>351</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="D22" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="E22" s="33" t="s">
         <v>353</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="F22" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>355</v>
+      </c>
+      <c r="H22" s="31"/>
       <c r="I22" s="19" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -6872,27 +6940,27 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>355</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>356</v>
-      </c>
-      <c r="E23" s="32" t="s">
+      <c r="B23" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="D23" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="E23" s="33" t="s">
         <v>359</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="F23" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="G23" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="H23" s="31"/>
       <c r="I23" s="19" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -6913,28 +6981,28 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="36" t="s">
-        <v>361</v>
-      </c>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
@@ -6990,19 +7058,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7027,20 +7095,20 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="C2" s="37" t="str">
+        <v>370</v>
+      </c>
+      <c r="C2" s="38" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-26 12-17</v>
+        <v xml:space="preserve">2023-01-06 10-03</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>

</xml_diff>

<commit_message>
Update default config to only set `create` if a phone number is provided
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -621,7 +621,7 @@
     <t>create</t>
   </si>
   <si>
-    <t xml:space="preserve">selected( ${role},'chw') or selected( ${role},'chw_supervisor')</t>
+    <t xml:space="preserve">${phone} != '' and (selected( ${role},'chw') or selected( ${role},'chw_supervisor'))</t>
   </si>
   <si>
     <t>meta</t>
@@ -1149,31 +1149,31 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
     </font>
     <font>
+      <sz val="10.000000"/>
       <name val="Arial"/>
-      <sz val="10.000000"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b/>
       <sz val="11.000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.000000"/>
       <name val="Calibri"/>
-      <sz val="11.000000"/>
     </font>
     <font>
+      <sz val="11.000000"/>
       <name val="Arial"/>
-      <sz val="11.000000"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1261,7 +1261,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1295,7 +1295,10 @@
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf fontId="3" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="5" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
@@ -4759,7 +4762,7 @@
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="24" t="s">
+      <c r="P50" s="25" t="s">
         <v>200</v>
       </c>
       <c r="Q50" s="16"/>
@@ -5250,7 +5253,7 @@
       <c r="AR59" s="16"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="17" t="s">
@@ -5314,7 +5317,7 @@
       <c r="AR60" s="16"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="17" t="s">
@@ -6090,13 +6093,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -6136,28 +6139,28 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="29" t="s">
         <v>227</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="31"/>
+      <c r="H2" s="32"/>
       <c r="I2" s="19" t="s">
         <v>231</v>
       </c>
@@ -6180,28 +6183,28 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="29" t="s">
         <v>234</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="H3" s="31"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="19" t="s">
         <v>238</v>
       </c>
@@ -6224,28 +6227,28 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="H4" s="31"/>
+      <c r="H4" s="32"/>
       <c r="I4" s="19" t="s">
         <v>246</v>
       </c>
@@ -6268,28 +6271,28 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="32"/>
       <c r="I5" s="19" t="s">
         <v>253</v>
       </c>
@@ -6312,28 +6315,28 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="H6" s="31"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="19" t="s">
         <v>260</v>
       </c>
@@ -6356,28 +6359,28 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="H7" s="31"/>
+      <c r="H7" s="32"/>
       <c r="I7" s="19" t="s">
         <v>267</v>
       </c>
@@ -6400,28 +6403,28 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="H8" s="31"/>
+      <c r="H8" s="32"/>
       <c r="I8" s="19" t="s">
         <v>274</v>
       </c>
@@ -6447,17 +6450,17 @@
       <c r="A9" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>276</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
       <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -6481,25 +6484,25 @@
       <c r="A10" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="30" t="s">
         <v>283</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="H10" s="31"/>
+      <c r="H10" s="32"/>
       <c r="I10" s="19" t="s">
         <v>285</v>
       </c>
@@ -6525,25 +6528,25 @@
       <c r="A11" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="30" t="s">
         <v>290</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="31" t="s">
         <v>291</v>
       </c>
-      <c r="H11" s="31"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="19" t="s">
         <v>292</v>
       </c>
@@ -6569,25 +6572,25 @@
       <c r="A12" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="30" t="s">
         <v>297</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="H12" s="31"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="19" t="s">
         <v>298</v>
       </c>
@@ -6613,25 +6616,25 @@
       <c r="A13" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="H13" s="31"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="19" t="s">
         <v>305</v>
       </c>
@@ -6663,19 +6666,19 @@
       <c r="C14" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="H14" s="31"/>
+      <c r="H14" s="32"/>
       <c r="I14" s="19" t="s">
         <v>307</v>
       </c>
@@ -6701,25 +6704,25 @@
       <c r="A15" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="35" t="s">
         <v>312</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="H15" s="31"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="19" t="s">
         <v>317</v>
       </c>
@@ -6742,28 +6745,28 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="29" t="s">
         <v>227</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="H16" s="31"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="19" t="s">
         <v>231</v>
       </c>
@@ -6786,28 +6789,28 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="H17" s="31"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="19" t="s">
         <v>325</v>
       </c>
@@ -6833,25 +6836,25 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="31" t="s">
         <v>331</v>
       </c>
-      <c r="H18" s="31"/>
+      <c r="H18" s="32"/>
       <c r="I18" s="19" t="s">
         <v>332</v>
       </c>
@@ -6877,25 +6880,25 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="34" t="s">
         <v>336</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="H19" s="31"/>
+      <c r="H19" s="32"/>
       <c r="I19" s="19" t="s">
         <v>339</v>
       </c>
@@ -6921,25 +6924,25 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="36" t="s">
         <v>341</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="29" t="s">
         <v>342</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="34" t="s">
         <v>343</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="30" t="s">
         <v>344</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="31" t="s">
         <v>342</v>
       </c>
-      <c r="H20" s="31"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="19" t="s">
         <v>345</v>
       </c>
@@ -6965,25 +6968,25 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="H21" s="31"/>
+      <c r="H21" s="32"/>
       <c r="I21" s="19" t="s">
         <v>351</v>
       </c>
@@ -7009,25 +7012,25 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="31" t="s">
         <v>356</v>
       </c>
-      <c r="H22" s="31"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="19" t="s">
         <v>357</v>
       </c>
@@ -7053,25 +7056,25 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="34" t="s">
         <v>360</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G23" s="37" t="s">
         <v>362</v>
       </c>
-      <c r="H23" s="31"/>
+      <c r="H23" s="32"/>
       <c r="I23" s="19" t="s">
         <v>363</v>
       </c>
@@ -7094,28 +7097,28 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="38" t="s">
         <v>364</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="31"/>
+      <c r="H24" s="32"/>
       <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
@@ -7213,9 +7216,9 @@
       <c r="B2" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="C2" s="38" t="str">
+      <c r="C2" s="39" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2023-01-26 16-02</v>
+        <v xml:space="preserve">2023-02-14 7-41</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>372</v>

</xml_diff>

<commit_message>
feat: add support for auto-creating users for new contacts (#7988)
Co-authored-by: Joshua Kuestersteffen <jkuester@kuester7.com>
Co-authored-by: Tatiana Lépiz <94494491+tatilepizs@users.noreply.github.com>

Closes #7753
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/PLACE_TYPE-create.xlsx
+++ b/config/default/forms/contact/PLACE_TYPE-create.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="374">
   <si>
     <t>type</t>
   </si>
@@ -613,6 +613,15 @@
   </si>
   <si>
     <t>multiline</t>
+  </si>
+  <si>
+    <t>user_for_contact</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${phone} != '' and (selected( ${role},'chw') or selected( ${role},'chw_supervisor'))</t>
   </si>
   <si>
     <t>meta</t>
@@ -1138,28 +1147,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
     </font>
     <font>
+      <sz val="10.000000"/>
       <name val="Arial"/>
-      <sz val="10.000000"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b/>
       <sz val="11.000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.000000"/>
       <name val="Calibri"/>
-      <sz val="11.000000"/>
     </font>
     <font>
+      <sz val="11.000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.000000"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1247,7 +1261,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1275,12 +1289,20 @@
     </xf>
     <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="4" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="3" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="3" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="5" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1">
+      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3665,7 +3687,7 @@
       </c>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
-      <c r="N32" s="21" t="s">
+      <c r="N32" s="16" t="s">
         <v>117</v>
       </c>
       <c r="O32" s="16" t="s">
@@ -4003,7 +4025,7 @@
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
-      <c r="P38" s="22" t="s">
+      <c r="P38" s="21" t="s">
         <v>141</v>
       </c>
       <c r="Q38" s="16"/>
@@ -4096,7 +4118,7 @@
       <c r="B40" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>145</v>
       </c>
       <c r="D40" s="18"/>
@@ -4224,7 +4246,7 @@
       </c>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
-      <c r="N42" s="23" t="b">
+      <c r="N42" s="22" t="b">
         <f t="shared" ref="N42:N43" si="0">TRUE()</f>
         <v>1</v>
       </c>
@@ -4293,7 +4315,7 @@
       </c>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
-      <c r="N43" s="23" t="b">
+      <c r="N43" s="22" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4659,26 +4681,34 @@
       <c r="AR48" s="16"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="16"/>
+      <c r="D49" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24" t="s">
+        <v>28</v>
+      </c>
       <c r="J49" s="16"/>
       <c r="K49" s="16"/>
-      <c r="L49" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
       <c r="O49" s="16"/>
@@ -4713,10 +4743,10 @@
       <c r="AR49" s="16"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="23" t="s">
         <v>199</v>
       </c>
       <c r="C50" s="16"/>
@@ -4732,7 +4762,7 @@
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
       <c r="O50" s="16"/>
-      <c r="P50" s="16" t="s">
+      <c r="P50" s="25" t="s">
         <v>200</v>
       </c>
       <c r="Q50" s="16"/>
@@ -4765,12 +4795,10 @@
       <c r="AR50" s="16"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>201</v>
-      </c>
+      <c r="A51" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="23"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
@@ -4784,9 +4812,7 @@
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
       <c r="O51" s="16"/>
-      <c r="P51" s="16" t="s">
-        <v>202</v>
-      </c>
+      <c r="P51" s="16"/>
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
       <c r="S51" s="16"/>
@@ -4818,12 +4844,14 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="C52" s="16"/>
+        <v>201</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
       <c r="F52" s="16"/>
@@ -4832,13 +4860,13 @@
       <c r="I52" s="16"/>
       <c r="J52" s="16"/>
       <c r="K52" s="16"/>
-      <c r="L52" s="16"/>
+      <c r="L52" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M52" s="16"/>
       <c r="N52" s="16"/>
       <c r="O52" s="16"/>
-      <c r="P52" s="16" t="s">
-        <v>204</v>
-      </c>
+      <c r="P52" s="16"/>
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
       <c r="S52" s="16"/>
@@ -4870,9 +4898,11 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>202</v>
+      </c>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
@@ -4886,7 +4916,9 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
       <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
+      <c r="P53" s="16" t="s">
+        <v>203</v>
+      </c>
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
       <c r="S53" s="16"/>
@@ -4918,9 +4950,11 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
@@ -4934,7 +4968,9 @@
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
       <c r="O54" s="16"/>
-      <c r="P54" s="16"/>
+      <c r="P54" s="16" t="s">
+        <v>205</v>
+      </c>
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
       <c r="S54" s="16"/>
@@ -4965,76 +5001,72 @@
       <c r="AR54" s="16"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="15"/>
+      <c r="A55" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
       <c r="I55" s="16"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="8"/>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="12"/>
-      <c r="U55" s="13"/>
-      <c r="V55" s="14"/>
-      <c r="W55" s="15"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="16"/>
+      <c r="V55" s="16"/>
+      <c r="W55" s="16"/>
       <c r="X55" s="16"/>
-      <c r="Y55" s="8"/>
-      <c r="Z55" s="8"/>
-      <c r="AA55" s="8"/>
-      <c r="AB55" s="8"/>
-      <c r="AC55" s="8"/>
-      <c r="AD55" s="8"/>
-      <c r="AE55" s="8"/>
-      <c r="AF55" s="8"/>
-      <c r="AG55" s="8"/>
-      <c r="AH55" s="8"/>
-      <c r="AI55" s="8"/>
-      <c r="AJ55" s="8"/>
-      <c r="AK55" s="8"/>
-      <c r="AL55" s="8"/>
+      <c r="Y55" s="16"/>
+      <c r="Z55" s="16"/>
+      <c r="AA55" s="16"/>
+      <c r="AB55" s="16"/>
+      <c r="AC55" s="16"/>
+      <c r="AD55" s="16"/>
+      <c r="AE55" s="16"/>
+      <c r="AF55" s="16"/>
+      <c r="AG55" s="16"/>
+      <c r="AH55" s="16"/>
+      <c r="AI55" s="16"/>
+      <c r="AJ55" s="16"/>
+      <c r="AK55" s="16"/>
+      <c r="AL55" s="16"/>
+      <c r="AM55" s="16"/>
+      <c r="AN55" s="16"/>
+      <c r="AO55" s="16"/>
+      <c r="AP55" s="16"/>
+      <c r="AQ55" s="16"/>
+      <c r="AR55" s="16"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>28</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B56" s="17"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
       <c r="H56" s="16"/>
-      <c r="I56" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I56" s="16"/>
       <c r="J56" s="16"/>
       <c r="K56" s="16"/>
-      <c r="L56" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="L56" s="16"/>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
       <c r="O56" s="16"/>
@@ -5069,31 +5101,17 @@
       <c r="AR56" s="16"/>
     </row>
     <row r="57" ht="14.25" customHeight="1">
-      <c r="A57" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F57" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="A57" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="17"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
       <c r="H57" s="16"/>
-      <c r="I57" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="I57" s="16"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16"/>
       <c r="L57" s="16"/>
@@ -5109,9 +5127,7 @@
       <c r="V57" s="16"/>
       <c r="W57" s="16"/>
       <c r="X57" s="16"/>
-      <c r="Y57" s="16" t="s">
-        <v>94</v>
-      </c>
+      <c r="Y57" s="16"/>
       <c r="Z57" s="16"/>
       <c r="AA57" s="16"/>
       <c r="AB57" s="16"/>
@@ -5133,101 +5149,75 @@
       <c r="AR57" s="16"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
-      <c r="A58" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F58" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="16"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="16"/>
-      <c r="O58" s="16"/>
-      <c r="P58" s="16"/>
-      <c r="Q58" s="16"/>
-      <c r="R58" s="16"/>
-      <c r="S58" s="16"/>
-      <c r="T58" s="16"/>
-      <c r="U58" s="16"/>
-      <c r="V58" s="16"/>
-      <c r="W58" s="16"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="12"/>
+      <c r="U58" s="13"/>
+      <c r="V58" s="14"/>
+      <c r="W58" s="15"/>
       <c r="X58" s="16"/>
-      <c r="Y58" s="16"/>
-      <c r="Z58" s="16"/>
-      <c r="AA58" s="16"/>
-      <c r="AB58" s="16"/>
-      <c r="AC58" s="16"/>
-      <c r="AD58" s="16"/>
-      <c r="AE58" s="16"/>
-      <c r="AF58" s="16"/>
-      <c r="AG58" s="16"/>
-      <c r="AH58" s="16"/>
-      <c r="AI58" s="16"/>
-      <c r="AJ58" s="16"/>
-      <c r="AK58" s="16"/>
-      <c r="AL58" s="16"/>
-      <c r="AM58" s="16"/>
-      <c r="AN58" s="16"/>
-      <c r="AO58" s="16"/>
-      <c r="AP58" s="16"/>
-      <c r="AQ58" s="16"/>
-      <c r="AR58" s="16"/>
+      <c r="Y58" s="8"/>
+      <c r="Z58" s="8"/>
+      <c r="AA58" s="8"/>
+      <c r="AB58" s="8"/>
+      <c r="AC58" s="8"/>
+      <c r="AD58" s="8"/>
+      <c r="AE58" s="8"/>
+      <c r="AF58" s="8"/>
+      <c r="AG58" s="8"/>
+      <c r="AH58" s="8"/>
+      <c r="AI58" s="8"/>
+      <c r="AJ58" s="8"/>
+      <c r="AK58" s="8"/>
+      <c r="AL58" s="8"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="17" t="s">
-        <v>205</v>
+        <v>26</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>207</v>
+        <v>28</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>209</v>
+        <v>28</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>210</v>
+        <v>28</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>211</v>
+        <v>28</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="J59" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K59" s="16" t="s">
-        <v>213</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
       <c r="L59" s="16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="M59" s="16"/>
       <c r="N59" s="16"/>
@@ -5241,9 +5231,7 @@
       <c r="V59" s="16"/>
       <c r="W59" s="16"/>
       <c r="X59" s="16"/>
-      <c r="Y59" s="16" t="s">
-        <v>214</v>
-      </c>
+      <c r="Y59" s="16"/>
       <c r="Z59" s="16"/>
       <c r="AA59" s="16"/>
       <c r="AB59" s="16"/>
@@ -5265,42 +5253,38 @@
       <c r="AR59" s="16"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="17" t="s">
-        <v>59</v>
+      <c r="A60" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>97</v>
+        <v>28</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>98</v>
+        <v>28</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="J60" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J60" s="16"/>
       <c r="K60" s="16"/>
       <c r="L60" s="16"/>
       <c r="M60" s="16"/>
       <c r="N60" s="16"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="16" t="s">
-        <v>216</v>
-      </c>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
       <c r="S60" s="16"/>
@@ -5309,7 +5293,9 @@
       <c r="V60" s="16"/>
       <c r="W60" s="16"/>
       <c r="X60" s="16"/>
-      <c r="Y60" s="16"/>
+      <c r="Y60" s="16" t="s">
+        <v>94</v>
+      </c>
       <c r="Z60" s="16"/>
       <c r="AA60" s="16"/>
       <c r="AB60" s="16"/>
@@ -5331,30 +5317,30 @@
       <c r="AR60" s="16"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
-      <c r="A61" s="17" t="s">
-        <v>30</v>
+      <c r="A61" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>185</v>
+        <v>0</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>187</v>
+        <v>28</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>188</v>
+        <v>28</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="G61" s="18" t="s">
-        <v>190</v>
+        <v>28</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16" t="s">
-        <v>191</v>
+        <v>28</v>
       </c>
       <c r="J61" s="16"/>
       <c r="K61" s="16"/>
@@ -5394,34 +5380,38 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="17" t="s">
-        <v>30</v>
+        <v>208</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="G62" s="18" t="s">
-        <v>196</v>
+        <v>213</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>214</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="J62" s="16"/>
-      <c r="K62" s="16"/>
+        <v>215</v>
+      </c>
+      <c r="J62" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="K62" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="L62" s="16" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
       <c r="M62" s="16"/>
       <c r="N62" s="16"/>
@@ -5435,7 +5425,9 @@
       <c r="V62" s="16"/>
       <c r="W62" s="16"/>
       <c r="X62" s="16"/>
-      <c r="Y62" s="16"/>
+      <c r="Y62" s="16" t="s">
+        <v>217</v>
+      </c>
       <c r="Z62" s="16"/>
       <c r="AA62" s="16"/>
       <c r="AB62" s="16"/>
@@ -5461,23 +5453,37 @@
         <v>59</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
+        <v>1</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>97</v>
+      </c>
       <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
+      <c r="I63" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="K63" s="16"/>
       <c r="L63" s="16"/>
       <c r="M63" s="16"/>
       <c r="N63" s="16"/>
-      <c r="O63" s="16"/>
+      <c r="O63" s="21"/>
       <c r="P63" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
@@ -5510,27 +5516,37 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="17" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
+        <v>185</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>190</v>
+      </c>
       <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
+      <c r="I64" s="16" t="s">
+        <v>191</v>
+      </c>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>
       <c r="M64" s="16"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
-      <c r="P64" s="16" t="s">
-        <v>220</v>
-      </c>
+      <c r="P64" s="16"/>
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
       <c r="S64" s="16"/>
@@ -5562,34 +5578,34 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>28</v>
+        <v>195</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>28</v>
+        <v>196</v>
       </c>
       <c r="H65" s="16"/>
       <c r="I65" s="16" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
       <c r="L65" s="16" t="s">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="M65" s="16"/>
       <c r="N65" s="16"/>
@@ -5629,7 +5645,7 @@
         <v>59</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="C66" s="16"/>
       <c r="D66" s="16"/>
@@ -5645,7 +5661,7 @@
       <c r="N66" s="16"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="Q66" s="16"/>
       <c r="R66" s="16"/>
@@ -5681,7 +5697,7 @@
         <v>59</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="C67" s="16"/>
       <c r="D67" s="16"/>
@@ -5697,7 +5713,7 @@
       <c r="N67" s="16"/>
       <c r="O67" s="16"/>
       <c r="P67" s="16" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="Q67" s="16"/>
       <c r="R67" s="16"/>
@@ -5730,27 +5746,39 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="17" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
+        <v>201</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="H68" s="16"/>
-      <c r="I68" s="16"/>
+      <c r="I68" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
-      <c r="L68" s="16"/>
+      <c r="L68" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="M68" s="16"/>
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
-      <c r="P68" s="16" t="s">
-        <v>204</v>
-      </c>
+      <c r="P68" s="16"/>
       <c r="Q68" s="16"/>
       <c r="R68" s="16"/>
       <c r="S68" s="16"/>
@@ -5782,9 +5810,11 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>202</v>
+      </c>
       <c r="C69" s="16"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
@@ -5798,7 +5828,9 @@
       <c r="M69" s="16"/>
       <c r="N69" s="16"/>
       <c r="O69" s="16"/>
-      <c r="P69" s="16"/>
+      <c r="P69" s="16" t="s">
+        <v>203</v>
+      </c>
       <c r="Q69" s="16"/>
       <c r="R69" s="16"/>
       <c r="S69" s="16"/>
@@ -5830,9 +5862,11 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B70" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="C70" s="16"/>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
@@ -5846,7 +5880,9 @@
       <c r="M70" s="16"/>
       <c r="N70" s="16"/>
       <c r="O70" s="16"/>
-      <c r="P70" s="16"/>
+      <c r="P70" s="16" t="s">
+        <v>205</v>
+      </c>
       <c r="Q70" s="16"/>
       <c r="R70" s="16"/>
       <c r="S70" s="16"/>
@@ -5875,6 +5911,154 @@
       <c r="AP70" s="16"/>
       <c r="AQ70" s="16"/>
       <c r="AR70" s="16"/>
+    </row>
+    <row r="71" ht="14.25" customHeight="1">
+      <c r="A71" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
+      <c r="M71" s="16"/>
+      <c r="N71" s="16"/>
+      <c r="O71" s="16"/>
+      <c r="P71" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q71" s="16"/>
+      <c r="R71" s="16"/>
+      <c r="S71" s="16"/>
+      <c r="T71" s="16"/>
+      <c r="U71" s="16"/>
+      <c r="V71" s="16"/>
+      <c r="W71" s="16"/>
+      <c r="X71" s="16"/>
+      <c r="Y71" s="16"/>
+      <c r="Z71" s="16"/>
+      <c r="AA71" s="16"/>
+      <c r="AB71" s="16"/>
+      <c r="AC71" s="16"/>
+      <c r="AD71" s="16"/>
+      <c r="AE71" s="16"/>
+      <c r="AF71" s="16"/>
+      <c r="AG71" s="16"/>
+      <c r="AH71" s="16"/>
+      <c r="AI71" s="16"/>
+      <c r="AJ71" s="16"/>
+      <c r="AK71" s="16"/>
+      <c r="AL71" s="16"/>
+      <c r="AM71" s="16"/>
+      <c r="AN71" s="16"/>
+      <c r="AO71" s="16"/>
+      <c r="AP71" s="16"/>
+      <c r="AQ71" s="16"/>
+      <c r="AR71" s="16"/>
+    </row>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B72" s="17"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
+      <c r="K72" s="16"/>
+      <c r="L72" s="16"/>
+      <c r="M72" s="16"/>
+      <c r="N72" s="16"/>
+      <c r="O72" s="16"/>
+      <c r="P72" s="16"/>
+      <c r="Q72" s="16"/>
+      <c r="R72" s="16"/>
+      <c r="S72" s="16"/>
+      <c r="T72" s="16"/>
+      <c r="U72" s="16"/>
+      <c r="V72" s="16"/>
+      <c r="W72" s="16"/>
+      <c r="X72" s="16"/>
+      <c r="Y72" s="16"/>
+      <c r="Z72" s="16"/>
+      <c r="AA72" s="16"/>
+      <c r="AB72" s="16"/>
+      <c r="AC72" s="16"/>
+      <c r="AD72" s="16"/>
+      <c r="AE72" s="16"/>
+      <c r="AF72" s="16"/>
+      <c r="AG72" s="16"/>
+      <c r="AH72" s="16"/>
+      <c r="AI72" s="16"/>
+      <c r="AJ72" s="16"/>
+      <c r="AK72" s="16"/>
+      <c r="AL72" s="16"/>
+      <c r="AM72" s="16"/>
+      <c r="AN72" s="16"/>
+      <c r="AO72" s="16"/>
+      <c r="AP72" s="16"/>
+      <c r="AQ72" s="16"/>
+      <c r="AR72" s="16"/>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="17"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
+      <c r="M73" s="16"/>
+      <c r="N73" s="16"/>
+      <c r="O73" s="16"/>
+      <c r="P73" s="16"/>
+      <c r="Q73" s="16"/>
+      <c r="R73" s="16"/>
+      <c r="S73" s="16"/>
+      <c r="T73" s="16"/>
+      <c r="U73" s="16"/>
+      <c r="V73" s="16"/>
+      <c r="W73" s="16"/>
+      <c r="X73" s="16"/>
+      <c r="Y73" s="16"/>
+      <c r="Z73" s="16"/>
+      <c r="AA73" s="16"/>
+      <c r="AB73" s="16"/>
+      <c r="AC73" s="16"/>
+      <c r="AD73" s="16"/>
+      <c r="AE73" s="16"/>
+      <c r="AF73" s="16"/>
+      <c r="AG73" s="16"/>
+      <c r="AH73" s="16"/>
+      <c r="AI73" s="16"/>
+      <c r="AJ73" s="16"/>
+      <c r="AK73" s="16"/>
+      <c r="AL73" s="16"/>
+      <c r="AM73" s="16"/>
+      <c r="AN73" s="16"/>
+      <c r="AO73" s="16"/>
+      <c r="AP73" s="16"/>
+      <c r="AQ73" s="16"/>
+      <c r="AR73" s="16"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -5909,13 +6093,13 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -5955,30 +6139,30 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>224</v>
+      <c r="A2" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>227</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>228</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="32"/>
       <c r="I2" s="19" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -5999,30 +6183,30 @@
       <c r="Z2" s="8"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>231</v>
+      <c r="A3" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>234</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="H3" s="30"/>
+        <v>235</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" s="32"/>
       <c r="I3" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -6043,30 +6227,30 @@
       <c r="Z3" s="8"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="B4" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="C4" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="D4" s="33" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="30"/>
+      <c r="E4" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="H4" s="32"/>
       <c r="I4" s="19" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -6087,30 +6271,30 @@
       <c r="Z4" s="8"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" s="32" t="s">
+      <c r="A5" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="C5" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="D5" s="33" t="s">
         <v>249</v>
       </c>
-      <c r="H5" s="30"/>
+      <c r="E5" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="H5" s="32"/>
       <c r="I5" s="19" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -6131,30 +6315,30 @@
       <c r="Z5" s="8"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="32" t="s">
+      <c r="B6" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="C6" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="D6" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="H6" s="30"/>
+      <c r="E6" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="H6" s="32"/>
       <c r="I6" s="19" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -6175,30 +6359,30 @@
       <c r="Z6" s="8"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="E7" s="32" t="s">
+      <c r="B7" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="C7" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="D7" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="H7" s="30"/>
+      <c r="E7" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" s="32"/>
       <c r="I7" s="19" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -6219,30 +6403,30 @@
       <c r="Z7" s="8"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="E8" s="32" t="s">
+      <c r="B8" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="C8" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="D8" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="E8" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="H8" s="32"/>
       <c r="I8" s="19" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -6264,19 +6448,19 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+        <v>275</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
       <c r="I9" s="19"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -6298,29 +6482,29 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>277</v>
-      </c>
-      <c r="D10" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="B10" s="35" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="C10" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="D10" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="H10" s="30"/>
+      <c r="E10" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="H10" s="32"/>
       <c r="I10" s="19" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -6342,29 +6526,29 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>284</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="E11" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="C11" s="36" t="s">
         <v>287</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="D11" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="H11" s="30"/>
+      <c r="E11" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="H11" s="32"/>
       <c r="I11" s="19" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -6386,29 +6570,29 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>291</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="E12" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>293</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="C12" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="G12" s="29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H12" s="30"/>
+      <c r="D12" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>295</v>
+      </c>
+      <c r="H12" s="32"/>
       <c r="I12" s="19" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -6430,29 +6614,29 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>298</v>
-      </c>
-      <c r="E13" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="35" t="s">
         <v>299</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="C13" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="D13" s="29" t="s">
         <v>301</v>
       </c>
-      <c r="H13" s="30"/>
+      <c r="E13" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>303</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="H13" s="32"/>
       <c r="I13" s="19" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -6474,29 +6658,29 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>306</v>
-      </c>
-      <c r="F14" s="28" t="s">
         <v>307</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="D14" s="29" t="s">
         <v>308</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="E14" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="H14" s="32"/>
       <c r="I14" s="19" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -6518,29 +6702,29 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="E15" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>312</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="C15" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="D15" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="H15" s="32"/>
       <c r="I15" s="19" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -6561,30 +6745,30 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>224</v>
+      <c r="A16" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>227</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="H16" s="30"/>
+        <v>228</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="H16" s="32"/>
       <c r="I16" s="19" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -6605,30 +6789,30 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="D17" s="27" t="s">
+      <c r="A17" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="F17" s="28" t="s">
+      <c r="B17" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="D17" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="H17" s="30"/>
+      <c r="E17" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="H17" s="32"/>
       <c r="I17" s="19" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -6652,27 +6836,27 @@
       <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>324</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>325</v>
-      </c>
-      <c r="E18" s="32" t="s">
+      <c r="B18" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="C18" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="D18" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="H18" s="30"/>
+      <c r="E18" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="H18" s="32"/>
       <c r="I18" s="19" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6696,27 +6880,27 @@
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>331</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>332</v>
-      </c>
-      <c r="E19" s="32" t="s">
+      <c r="B19" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="C19" s="36" t="s">
         <v>334</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="D19" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="E19" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>337</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>338</v>
+      </c>
+      <c r="H19" s="32"/>
       <c r="I19" s="19" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6740,27 +6924,27 @@
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>338</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="E20" s="32" t="s">
+      <c r="B20" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="C20" s="36" t="s">
         <v>341</v>
       </c>
-      <c r="G20" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="H20" s="30"/>
+      <c r="D20" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="H20" s="32"/>
       <c r="I20" s="19" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6784,27 +6968,27 @@
       <c r="A21" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>323</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>343</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>344</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>345</v>
-      </c>
-      <c r="F21" s="28" t="s">
+      <c r="B21" s="35" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="D21" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="H21" s="30"/>
+      <c r="E21" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="H21" s="32"/>
       <c r="I21" s="19" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6828,27 +7012,27 @@
       <c r="A22" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="C22" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>350</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="F22" s="28" t="s">
+      <c r="B22" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="D22" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="H22" s="30"/>
+      <c r="E22" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>355</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>356</v>
+      </c>
+      <c r="H22" s="32"/>
       <c r="I22" s="19" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -6872,27 +7056,27 @@
       <c r="A23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>337</v>
-      </c>
-      <c r="C23" s="34" t="s">
-        <v>355</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>356</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>357</v>
-      </c>
-      <c r="F23" s="28" t="s">
+      <c r="B23" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="C23" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="D23" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="E23" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="G23" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="H23" s="32"/>
       <c r="I23" s="19" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -6913,28 +7097,28 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="36" t="s">
-        <v>361</v>
-      </c>
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="29" t="s">
+      <c r="G24" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="30"/>
+      <c r="H24" s="32"/>
       <c r="I24" s="19" t="s">
         <v>100</v>
       </c>
@@ -6990,19 +7174,19 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7027,20 +7211,20 @@
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="C2" s="37" t="str">
+        <v>371</v>
+      </c>
+      <c r="C2" s="39" t="str">
         <f ca="1">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v xml:space="preserve">2022-09-26 12-17</v>
+        <v xml:space="preserve">2023-02-14 7-41</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>

</xml_diff>